<commit_message>
Changes as of 16/03/20 5:00PM
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="81">
   <si>
     <t xml:space="preserve">Test_Case_Name</t>
   </si>
@@ -85,6 +85,24 @@
     <t xml:space="preserve">Adactrain@1</t>
   </si>
   <si>
+    <t xml:space="preserve">User_is_able_to_book_a_hotel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iPhone_SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sydney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel Creek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 – One</t>
+  </si>
+  <si>
     <t xml:space="preserve">User_is_shown_an_error_message_when_any_mandatory_field_is_not_entered_and_he_clicks_on_the_search_button</t>
   </si>
   <si>
@@ -94,40 +112,25 @@
     <t xml:space="preserve">User_is_able_to_view_the_drop_down_list_in_locations</t>
   </si>
   <si>
-    <t xml:space="preserve">Sydney, Melbourne, Brisbane, Adelaide, London, New York, Los Angeles, Paris</t>
+    <t xml:space="preserve">Sydney,Melbourne,Brisbane,Adelaide, London,New York,Los Angeles,Paris</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_view_list_of_hotels_in_the_drop_down_menu_</t>
   </si>
   <si>
-    <t xml:space="preserve">Hotel Creek, 
-Hotel Sunshine, 
-Hotel Hervey, 
-Hotel Cornice</t>
+    <t xml:space="preserve">Hotel Creek,Hotel Sunshine,Hotel Hervey, Hotel Cornice</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_view_list_of_options_in_the_Room_Type_drop_down_menu</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard,
-Deluxe,
-Double,
-Super Deluxe</t>
+    <t xml:space="preserve">Standard,Deluxe,Double,Super Deluxe</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_view_the_list_of_options_in_the_Number_of_Rooms_drop_down_menu</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – One
-2 – Two
-3 – Three
-4 – Four
-5 – Five
-6 – Six
-7 – Seven
-8 – Eight
-9 – Nine
-10 - Ten</t>
+    <t xml:space="preserve">1 – One,2 – Two,3 – Three,4 – Four,5 – Five,6 – Six,7 – Seven,8 – Eight,9 – Nine,10 – Ten</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_enter_check_in_date_in_the_check_in_date_field</t>
@@ -151,13 +154,7 @@
     <t xml:space="preserve">User_is_able_to_view_the_list_in_the_Adults_per_Room_drop_down_menu</t>
   </si>
   <si>
-    <t xml:space="preserve">iPhone_SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 – One
-2 – Two
-3 – Three
-4 – Four</t>
+    <t xml:space="preserve">1 – One,2 – Two,3 – Three,4 – Four</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_view_Children_per_room_list_in_the_children_per_room_drop_down_menu</t>
@@ -188,9 +185,6 @@
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_view_the_details_of_the_hotel_selected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sydney</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_scroll_up_and_down_the_screen</t>
@@ -275,9 +269,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -415,6 +410,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -423,11 +422,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,10 +503,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,7 +517,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.65"/>
@@ -611,8 +606,8 @@
       <c r="H2" s="7"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -622,7 +617,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>13.3</v>
@@ -633,12 +628,34 @@
       <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>22</v>
+      <c r="H3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="9" t="n">
+        <v>43919</v>
+      </c>
+      <c r="M3" s="9" t="n">
+        <v>43920</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>16</v>
@@ -661,9 +678,9 @@
       <c r="H4" s="7"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>23</v>
+    <row r="5" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>16</v>
@@ -683,13 +700,12 @@
       <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="46.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>25</v>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>16</v>
@@ -709,14 +725,13 @@
       <c r="G6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="46.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>27</v>
+      <c r="H6" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>16</v>
@@ -736,13 +751,14 @@
       <c r="G7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="113.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>29</v>
+      <c r="H7" s="7"/>
+      <c r="I7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>16</v>
@@ -762,13 +778,13 @@
       <c r="G8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>31</v>
+      <c r="J8" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>16</v>
@@ -788,13 +804,13 @@
       <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="11" t="n">
-        <v>43919</v>
+      <c r="K9" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>32</v>
+      <c r="A10" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>16</v>
@@ -814,13 +830,13 @@
       <c r="G10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="11" t="n">
+      <c r="L10" s="9" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>33</v>
+      <c r="A11" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>16</v>
@@ -840,13 +856,13 @@
       <c r="G11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="11" t="n">
+      <c r="L11" s="9" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
+      <c r="A12" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>16</v>
@@ -866,13 +882,13 @@
       <c r="G12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="12" t="n">
-        <v>43920</v>
+      <c r="L12" s="9" t="n">
+        <v>43919</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>16</v>
@@ -892,13 +908,13 @@
       <c r="G13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="12" t="n">
+      <c r="M13" s="9" t="n">
         <v>43920</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>16</v>
@@ -918,13 +934,13 @@
       <c r="G14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M14" s="12" t="n">
+      <c r="M14" s="9" t="n">
         <v>43920</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="46.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>16</v>
@@ -933,7 +949,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>13.3</v>
@@ -944,13 +960,13 @@
       <c r="G15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="N15" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="46.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M15" s="9" t="n">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>16</v>
@@ -959,7 +975,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>13.3</v>
@@ -970,13 +986,13 @@
       <c r="G16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O16" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N16" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>16</v>
@@ -985,7 +1001,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>13.3</v>
@@ -995,11 +1011,14 @@
       </c>
       <c r="G17" s="7" t="s">
         <v>20</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>16</v>
@@ -1008,7 +1027,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>13.3</v>
@@ -1022,7 +1041,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>16</v>
@@ -1031,7 +1050,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>13.3</v>
@@ -1045,7 +1064,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>16</v>
@@ -1054,17 +1073,21 @@
         <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
+      <c r="F20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>16</v>
@@ -1073,15 +1096,17 @@
         <v>17</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>13.3</v>
       </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>16</v>
@@ -1090,21 +1115,15 @@
         <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13.3</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <v>123344</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>16</v>
@@ -1113,15 +1132,21 @@
         <v>17</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>13.3</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <v>123344</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>16</v>
@@ -1130,24 +1155,15 @@
         <v>17</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>13.3</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>16</v>
@@ -1156,7 +1172,7 @@
         <v>17</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>13.3</v>
@@ -1166,11 +1182,35 @@
       </c>
       <c r="G25" s="7" t="s">
         <v>20</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" s="12" t="n">
+        <v>43919</v>
+      </c>
+      <c r="M25" s="9" t="n">
+        <v>43920</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>16</v>
@@ -1179,7 +1219,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>13.3</v>
@@ -1193,7 +1233,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>16</v>
@@ -1202,7 +1242,7 @@
         <v>17</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>13.3</v>
@@ -1216,7 +1256,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>16</v>
@@ -1225,7 +1265,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>13.3</v>
@@ -1239,7 +1279,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>16</v>
@@ -1248,7 +1288,7 @@
         <v>17</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>13.3</v>
@@ -1262,7 +1302,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>16</v>
@@ -1271,7 +1311,7 @@
         <v>17</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>13.3</v>
@@ -1285,7 +1325,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>16</v>
@@ -1294,7 +1334,7 @@
         <v>17</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13.3</v>
@@ -1308,7 +1348,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>16</v>
@@ -1317,7 +1357,7 @@
         <v>17</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13.3</v>
@@ -1329,9 +1369,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>16</v>
@@ -1340,7 +1380,7 @@
         <v>17</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>13.3</v>
@@ -1352,9 +1392,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>16</v>
@@ -1363,7 +1403,7 @@
         <v>17</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>13.3</v>
@@ -1377,7 +1417,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>16</v>
@@ -1386,7 +1426,7 @@
         <v>17</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13.3</v>
@@ -1400,7 +1440,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>16</v>
@@ -1409,7 +1449,7 @@
         <v>17</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13.3</v>
@@ -1423,7 +1463,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>16</v>
@@ -1432,7 +1472,7 @@
         <v>17</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>13.3</v>
@@ -1442,14 +1482,11 @@
       </c>
       <c r="G37" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>16</v>
@@ -1458,7 +1495,7 @@
         <v>17</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>13.3</v>
@@ -1470,12 +1507,12 @@
         <v>20</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>16</v>
@@ -1484,7 +1521,7 @@
         <v>17</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>13.3</v>
@@ -1495,13 +1532,13 @@
       <c r="G39" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="0" t="s">
-        <v>68</v>
+      <c r="H39" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>16</v>
@@ -1510,7 +1547,7 @@
         <v>17</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>13.3</v>
@@ -1520,11 +1557,14 @@
       </c>
       <c r="G40" s="7" t="s">
         <v>20</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>16</v>
@@ -1533,7 +1573,7 @@
         <v>17</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>13.3</v>
@@ -1543,14 +1583,11 @@
       </c>
       <c r="G41" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>16</v>
@@ -1559,7 +1596,7 @@
         <v>17</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>13.3</v>
@@ -1569,11 +1606,14 @@
       </c>
       <c r="G42" s="7" t="s">
         <v>20</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>16</v>
@@ -1582,7 +1622,7 @@
         <v>17</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>13.3</v>
@@ -1596,7 +1636,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>16</v>
@@ -1605,7 +1645,7 @@
         <v>17</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>13.3</v>
@@ -1619,7 +1659,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>16</v>
@@ -1628,7 +1668,7 @@
         <v>17</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13.3</v>
@@ -1642,7 +1682,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>16</v>
@@ -1651,7 +1691,7 @@
         <v>17</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13.3</v>
@@ -1665,7 +1705,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>16</v>
@@ -1674,7 +1714,7 @@
         <v>17</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13.3</v>
@@ -1683,6 +1723,29 @@
         <v>19</v>
       </c>
       <c r="G47" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1706,7 +1769,7 @@
     <hyperlink ref="G17" r:id="rId16" display="Adactrain@1"/>
     <hyperlink ref="G18" r:id="rId17" display="Adactrain@1"/>
     <hyperlink ref="G19" r:id="rId18" display="Adactrain@1"/>
-    <hyperlink ref="G24" r:id="rId19" display="Adactrain@1"/>
+    <hyperlink ref="G20" r:id="rId19" display="Adactrain@1"/>
     <hyperlink ref="G25" r:id="rId20" display="Adactrain@1"/>
     <hyperlink ref="G26" r:id="rId21" display="Adactrain@1"/>
     <hyperlink ref="G27" r:id="rId22" display="Adactrain@1"/>
@@ -1730,6 +1793,7 @@
     <hyperlink ref="G45" r:id="rId40" display="Adactrain@1"/>
     <hyperlink ref="G46" r:id="rId41" display="Adactrain@1"/>
     <hyperlink ref="G47" r:id="rId42" display="Adactrain@1"/>
+    <hyperlink ref="G48" r:id="rId43" display="Adactrain@1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Commiting new scroll method to scroll within the page and changes within the Search hotel method
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="82">
   <si>
     <t xml:space="preserve">Test_Case_Name</t>
   </si>
@@ -100,7 +100,33 @@
     <t xml:space="preserve">Standard</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – One</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> One</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">User_is_shown_an_error_message_when_any_mandatory_field_is_not_entered_and_he_clicks_on_the_search_button</t>
@@ -130,7 +156,177 @@
     <t xml:space="preserve">User_is_able_to_view_the_list_of_options_in_the_Number_of_Rooms_drop_down_menu</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – One,2 – Two,3 – Three,4 – Four,5 – Five,6 – Six,7 – Seven,8 – Eight,9 – Nine,10 – Ten</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1 - One,2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Two,3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Three,4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Four,5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Five,6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Six,7 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Seven,8 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Eight,9 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Nine,10 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Ten</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_enter_check_in_date_in_the_check_in_date_field</t>
@@ -154,10 +350,83 @@
     <t xml:space="preserve">User_is_able_to_view_the_list_in_the_Adults_per_Room_drop_down_menu</t>
   </si>
   <si>
-    <t xml:space="preserve">1 – One,2 – Two,3 – Three,4 – Four</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> One,2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- Two,3 - Three,4 - Four</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_view_Children_per_room_list_in_the_children_per_room_drop_down_menu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> One,2 –</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Two,3 - Three,4 - Four</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_click_on_the_search_button</t>
@@ -269,12 +538,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -320,6 +588,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF2A00FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -422,8 +696,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -505,8 +779,8 @@
   </sheetPr>
   <dimension ref="A1:S48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M25" activeCellId="0" sqref="M25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -606,7 +880,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>21</v>
       </c>
@@ -782,7 +1056,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="68.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>35</v>
       </c>
@@ -804,7 +1078,7 @@
       <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="12" t="s">
         <v>36</v>
       </c>
     </row>
@@ -964,7 +1238,7 @@
         <v>43920</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -990,7 +1264,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -1013,12 +1287,12 @@
         <v>20</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>16</v>
@@ -1041,7 +1315,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>16</v>
@@ -1064,7 +1338,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>16</v>
@@ -1087,7 +1361,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>16</v>
@@ -1106,7 +1380,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>16</v>
@@ -1123,7 +1397,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>16</v>
@@ -1138,7 +1412,7 @@
         <v>13.3</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>123344</v>
@@ -1146,7 +1420,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>16</v>
@@ -1161,9 +1435,9 @@
         <v>13.3</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>16</v>
@@ -1195,7 +1469,7 @@
       <c r="K25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L25" s="12" t="n">
+      <c r="L25" s="9" t="n">
         <v>43919</v>
       </c>
       <c r="M25" s="9" t="n">
@@ -1210,7 +1484,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>16</v>
@@ -1233,7 +1507,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>16</v>
@@ -1256,7 +1530,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>16</v>
@@ -1279,7 +1553,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>16</v>
@@ -1302,7 +1576,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>16</v>
@@ -1325,7 +1599,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>16</v>
@@ -1348,7 +1622,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>16</v>
@@ -1371,7 +1645,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>16</v>
@@ -1394,7 +1668,7 @@
     </row>
     <row r="34" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>16</v>
@@ -1417,7 +1691,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>16</v>
@@ -1440,7 +1714,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>16</v>
@@ -1463,7 +1737,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>16</v>
@@ -1486,7 +1760,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>16</v>
@@ -1507,12 +1781,12 @@
         <v>20</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>16</v>
@@ -1533,12 +1807,12 @@
         <v>20</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>16</v>
@@ -1559,12 +1833,12 @@
         <v>20</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>16</v>
@@ -1587,7 +1861,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>16</v>
@@ -1608,12 +1882,12 @@
         <v>20</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>16</v>
@@ -1636,7 +1910,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>16</v>
@@ -1659,7 +1933,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>16</v>
@@ -1682,7 +1956,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>16</v>
@@ -1705,7 +1979,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>16</v>
@@ -1728,7 +2002,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Committed as of 18/03/20
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="95">
   <si>
     <t xml:space="preserve">Test_Case_Name</t>
   </si>
@@ -67,6 +67,27 @@
     <t xml:space="preserve">Children per Room</t>
   </si>
   <si>
+    <t xml:space="preserve">First Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Billing Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC Expiry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVV</t>
+  </si>
+  <si>
     <t xml:space="preserve">User_is_able_to_login_into_the_application</t>
   </si>
   <si>
@@ -91,6 +112,12 @@
     <t xml:space="preserve">iPhone_SE</t>
   </si>
   <si>
+    <t xml:space="preserve">testusersbin6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testpw123)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sydney</t>
   </si>
   <si>
@@ -127,6 +154,18 @@
       </rPr>
       <t xml:space="preserve"> One</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">testuser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testuser12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billing address of test user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VISA</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_shown_an_error_message_when_any_mandatory_field_is_not_entered_and_he_clicks_on_the_search_button</t>
@@ -538,9 +577,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0000000000000000"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -647,7 +688,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -689,11 +730,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -777,10 +826,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S48"/>
+  <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -801,7 +850,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,69 +901,86 @@
       <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="L3" s="9" t="n">
         <v>43919</v>
@@ -921,240 +989,258 @@
         <v>43920</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" s="11" t="n">
+        <v>1234567891234570</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>1223</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>27</v>
+      <c r="A4" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>28</v>
+      <c r="A5" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
-        <v>29</v>
+      <c r="A6" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>31</v>
+      <c r="A7" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>33</v>
+      <c r="A8" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>34</v>
+        <v>27</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="68.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>35</v>
+      <c r="A9" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>37</v>
+      <c r="A10" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="L10" s="9" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>38</v>
+      <c r="A11" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="L11" s="9" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>39</v>
+      <c r="A12" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="L12" s="9" t="n">
         <v>43919</v>
@@ -1162,25 +1248,25 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="M13" s="9" t="n">
         <v>43920</v>
@@ -1188,25 +1274,25 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="M14" s="9" t="n">
         <v>43920</v>
@@ -1214,25 +1300,25 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="M15" s="9" t="n">
         <v>43920</v>
@@ -1240,137 +1326,137 @@
     </row>
     <row r="16" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>44</v>
+        <v>27</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O17" s="11" t="s">
-        <v>46</v>
+        <v>27</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>13.3</v>
@@ -1380,16 +1466,16 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13.3</v>
@@ -1397,22 +1483,22 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>123344</v>
@@ -1420,16 +1506,16 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>13.3</v>
@@ -1437,37 +1523,37 @@
     </row>
     <row r="25" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="L25" s="9" t="n">
         <v>43919</v>
@@ -1476,598 +1562,597 @@
         <v>43920</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="Adactrain@1"/>
-    <hyperlink ref="G3" r:id="rId2" display="Adactrain@1"/>
-    <hyperlink ref="G4" r:id="rId3" display="Adactrain@1"/>
-    <hyperlink ref="G5" r:id="rId4" display="Adactrain@1"/>
-    <hyperlink ref="G6" r:id="rId5" display="Adactrain@1"/>
-    <hyperlink ref="G7" r:id="rId6" display="Adactrain@1"/>
-    <hyperlink ref="G8" r:id="rId7" display="Adactrain@1"/>
-    <hyperlink ref="G9" r:id="rId8" display="Adactrain@1"/>
-    <hyperlink ref="G10" r:id="rId9" display="Adactrain@1"/>
-    <hyperlink ref="G11" r:id="rId10" display="Adactrain@1"/>
-    <hyperlink ref="G12" r:id="rId11" display="Adactrain@1"/>
-    <hyperlink ref="G13" r:id="rId12" display="Adactrain@1"/>
-    <hyperlink ref="G14" r:id="rId13" display="Adactrain@1"/>
-    <hyperlink ref="G15" r:id="rId14" display="Adactrain@1"/>
-    <hyperlink ref="G16" r:id="rId15" display="Adactrain@1"/>
-    <hyperlink ref="G17" r:id="rId16" display="Adactrain@1"/>
-    <hyperlink ref="G18" r:id="rId17" display="Adactrain@1"/>
-    <hyperlink ref="G19" r:id="rId18" display="Adactrain@1"/>
-    <hyperlink ref="G20" r:id="rId19" display="Adactrain@1"/>
-    <hyperlink ref="G25" r:id="rId20" display="Adactrain@1"/>
-    <hyperlink ref="G26" r:id="rId21" display="Adactrain@1"/>
-    <hyperlink ref="G27" r:id="rId22" display="Adactrain@1"/>
-    <hyperlink ref="G28" r:id="rId23" display="Adactrain@1"/>
-    <hyperlink ref="G29" r:id="rId24" display="Adactrain@1"/>
-    <hyperlink ref="G30" r:id="rId25" display="Adactrain@1"/>
-    <hyperlink ref="G31" r:id="rId26" display="Adactrain@1"/>
-    <hyperlink ref="G32" r:id="rId27" display="Adactrain@1"/>
-    <hyperlink ref="G33" r:id="rId28" display="Adactrain@1"/>
-    <hyperlink ref="G34" r:id="rId29" display="Adactrain@1"/>
-    <hyperlink ref="G35" r:id="rId30" display="Adactrain@1"/>
-    <hyperlink ref="G36" r:id="rId31" display="Adactrain@1"/>
-    <hyperlink ref="G37" r:id="rId32" display="Adactrain@1"/>
-    <hyperlink ref="G38" r:id="rId33" display="Adactrain@1"/>
-    <hyperlink ref="G39" r:id="rId34" display="Adactrain@1"/>
-    <hyperlink ref="G40" r:id="rId35" display="Adactrain@1"/>
-    <hyperlink ref="G41" r:id="rId36" display="Adactrain@1"/>
-    <hyperlink ref="G42" r:id="rId37" display="Adactrain@1"/>
-    <hyperlink ref="G43" r:id="rId38" display="Adactrain@1"/>
-    <hyperlink ref="G44" r:id="rId39" display="Adactrain@1"/>
-    <hyperlink ref="G45" r:id="rId40" display="Adactrain@1"/>
-    <hyperlink ref="G46" r:id="rId41" display="Adactrain@1"/>
-    <hyperlink ref="G47" r:id="rId42" display="Adactrain@1"/>
-    <hyperlink ref="G48" r:id="rId43" display="Adactrain@1"/>
+    <hyperlink ref="G4" r:id="rId2" display="Adactrain@1"/>
+    <hyperlink ref="G5" r:id="rId3" display="Adactrain@1"/>
+    <hyperlink ref="G6" r:id="rId4" display="Adactrain@1"/>
+    <hyperlink ref="G7" r:id="rId5" display="Adactrain@1"/>
+    <hyperlink ref="G8" r:id="rId6" display="Adactrain@1"/>
+    <hyperlink ref="G9" r:id="rId7" display="Adactrain@1"/>
+    <hyperlink ref="G10" r:id="rId8" display="Adactrain@1"/>
+    <hyperlink ref="G11" r:id="rId9" display="Adactrain@1"/>
+    <hyperlink ref="G12" r:id="rId10" display="Adactrain@1"/>
+    <hyperlink ref="G13" r:id="rId11" display="Adactrain@1"/>
+    <hyperlink ref="G14" r:id="rId12" display="Adactrain@1"/>
+    <hyperlink ref="G15" r:id="rId13" display="Adactrain@1"/>
+    <hyperlink ref="G16" r:id="rId14" display="Adactrain@1"/>
+    <hyperlink ref="G17" r:id="rId15" display="Adactrain@1"/>
+    <hyperlink ref="G18" r:id="rId16" display="Adactrain@1"/>
+    <hyperlink ref="G19" r:id="rId17" display="Adactrain@1"/>
+    <hyperlink ref="G20" r:id="rId18" display="Adactrain@1"/>
+    <hyperlink ref="G25" r:id="rId19" display="Adactrain@1"/>
+    <hyperlink ref="G26" r:id="rId20" display="Adactrain@1"/>
+    <hyperlink ref="G27" r:id="rId21" display="Adactrain@1"/>
+    <hyperlink ref="G28" r:id="rId22" display="Adactrain@1"/>
+    <hyperlink ref="G29" r:id="rId23" display="Adactrain@1"/>
+    <hyperlink ref="G30" r:id="rId24" display="Adactrain@1"/>
+    <hyperlink ref="G31" r:id="rId25" display="Adactrain@1"/>
+    <hyperlink ref="G32" r:id="rId26" display="Adactrain@1"/>
+    <hyperlink ref="G33" r:id="rId27" display="Adactrain@1"/>
+    <hyperlink ref="G34" r:id="rId28" display="Adactrain@1"/>
+    <hyperlink ref="G35" r:id="rId29" display="Adactrain@1"/>
+    <hyperlink ref="G36" r:id="rId30" display="Adactrain@1"/>
+    <hyperlink ref="G37" r:id="rId31" display="Adactrain@1"/>
+    <hyperlink ref="G38" r:id="rId32" display="Adactrain@1"/>
+    <hyperlink ref="G39" r:id="rId33" display="Adactrain@1"/>
+    <hyperlink ref="G40" r:id="rId34" display="Adactrain@1"/>
+    <hyperlink ref="G41" r:id="rId35" display="Adactrain@1"/>
+    <hyperlink ref="G42" r:id="rId36" display="Adactrain@1"/>
+    <hyperlink ref="G43" r:id="rId37" display="Adactrain@1"/>
+    <hyperlink ref="G44" r:id="rId38" display="Adactrain@1"/>
+    <hyperlink ref="G45" r:id="rId39" display="Adactrain@1"/>
+    <hyperlink ref="G46" r:id="rId40" display="Adactrain@1"/>
+    <hyperlink ref="G47" r:id="rId41" display="Adactrain@1"/>
+    <hyperlink ref="G48" r:id="rId42" display="Adactrain@1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Committing changes as of 19/03/20 4:33PM
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -112,7 +112,7 @@
     <t xml:space="preserve">iPhone_SE</t>
   </si>
   <si>
-    <t xml:space="preserve">testusersbin6</t>
+    <t xml:space="preserve">testusersbin13</t>
   </si>
   <si>
     <t xml:space="preserve">testpw123)</t>
@@ -579,9 +579,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="0000000000000000"/>
-    <numFmt numFmtId="167" formatCode="@"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="167" formatCode="0000000000000000"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -688,7 +688,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -725,7 +725,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -733,11 +737,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -828,8 +832,8 @@
   </sheetPr>
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -838,7 +842,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.32"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.13"/>
@@ -964,7 +968,7 @@
       <c r="E3" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -982,10 +986,10 @@
       <c r="K3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="9" t="n">
+      <c r="L3" s="10" t="n">
         <v>43919</v>
       </c>
-      <c r="M3" s="9" t="n">
+      <c r="M3" s="10" t="n">
         <v>43920</v>
       </c>
       <c r="N3" s="4" t="s">
@@ -1000,13 +1004,13 @@
       <c r="Q3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="R3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="11" t="n">
+      <c r="S3" s="12" t="n">
         <v>1234567891234570</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="13" t="s">
         <v>39</v>
       </c>
       <c r="V3" s="0" t="n">
@@ -1014,7 +1018,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1039,7 +1043,7 @@
       <c r="I4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1064,7 +1068,7 @@
       <c r="I5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1085,12 +1089,12 @@
       <c r="G6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1117,7 +1121,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1138,12 +1142,12 @@
       <c r="G8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="11" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="68.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>48</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1164,12 +1168,12 @@
       <c r="G9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1190,12 +1194,12 @@
       <c r="G10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="9" t="n">
+      <c r="L10" s="10" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -1216,12 +1220,12 @@
       <c r="G11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="9" t="n">
+      <c r="L11" s="10" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -1242,7 +1246,7 @@
       <c r="G12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="9" t="n">
+      <c r="L12" s="10" t="n">
         <v>43919</v>
       </c>
     </row>
@@ -1268,7 +1272,7 @@
       <c r="G13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M13" s="9" t="n">
+      <c r="M13" s="10" t="n">
         <v>43920</v>
       </c>
     </row>
@@ -1294,7 +1298,7 @@
       <c r="G14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M14" s="9" t="n">
+      <c r="M14" s="10" t="n">
         <v>43920</v>
       </c>
     </row>
@@ -1320,7 +1324,7 @@
       <c r="G15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M15" s="9" t="n">
+      <c r="M15" s="10" t="n">
         <v>43920</v>
       </c>
     </row>
@@ -1346,7 +1350,7 @@
       <c r="G16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N16" s="10" t="s">
+      <c r="N16" s="11" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1372,7 +1376,7 @@
       <c r="G17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="10" t="s">
+      <c r="O17" s="11" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1555,10 +1559,10 @@
       <c r="K25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L25" s="9" t="n">
+      <c r="L25" s="10" t="n">
         <v>43919</v>
       </c>
-      <c r="M25" s="9" t="n">
+      <c r="M25" s="10" t="n">
         <v>43920</v>
       </c>
       <c r="N25" s="4" t="s">

</xml_diff>

<commit_message>
committing new testcases to login and logout of the application
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="98">
   <si>
     <t xml:space="preserve">Test_Case_Name</t>
   </si>
@@ -88,6 +88,12 @@
     <t xml:space="preserve">CVV</t>
   </si>
   <si>
+    <t xml:space="preserve">Booked Itinerary id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email id</t>
+  </si>
+  <si>
     <t xml:space="preserve">User_is_able_to_login_into_the_application</t>
   </si>
   <si>
@@ -100,75 +106,78 @@
     <t xml:space="preserve">iPhone SE</t>
   </si>
   <si>
+    <t xml:space="preserve">testusersbin16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ED337V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_book_a_hotel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iPhone_SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sydney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel Creek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> One</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">testuser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testuser12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billing address of test user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VISA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_shown_an_error_message_when_any_mandatory_field_is_not_entered_and_he_clicks_on_the_search_button</t>
+  </si>
+  <si>
     <t xml:space="preserve">adactmobtest</t>
   </si>
   <si>
     <t xml:space="preserve">Adactrain@1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User_is_able_to_book_a_hotel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iPhone_SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testusersbin13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testpw123)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sydney</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hotel Creek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> One</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">testuser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testuser12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billing address of test user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VISA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User_is_shown_an_error_message_when_any_mandatory_field_is_not_entered_and_he_clicks_on_the_search_button</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_scroll_down_and_up_on_the_search_hotel_screen</t>
@@ -713,7 +722,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -723,10 +732,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -747,6 +752,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -830,10 +839,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -856,7 +865,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="20" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="17.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="24.6"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="25" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,1237 +938,1270 @@
       <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="G3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="10" t="n">
+      <c r="K4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="9" t="n">
         <v>43919</v>
       </c>
-      <c r="M3" s="10" t="n">
+      <c r="M4" s="9" t="n">
         <v>43920</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="0" t="s">
+      <c r="N4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="O4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="Q4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="12" t="n">
+      <c r="R4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" s="11" t="n">
         <v>1234567891234570</v>
       </c>
-      <c r="T3" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" s="0" t="n">
+      <c r="T4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="0" t="n">
         <v>1223</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="W4" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E5" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>26</v>
+      <c r="F5" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>42</v>
+    <row r="6" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>26</v>
+      <c r="F6" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>26</v>
+      <c r="F7" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E8" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>26</v>
+      <c r="F8" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="68.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E9" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>26</v>
+      <c r="F9" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="68.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="E10" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>26</v>
+      <c r="F10" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="10" t="n">
+      <c r="E11" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="9" t="n">
         <v>43919</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="7" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="10" t="n">
+      <c r="E12" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="9" t="n">
         <v>43919</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="7" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="10" t="n">
+      <c r="E13" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="9" t="n">
         <v>43919</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" s="10" t="n">
-        <v>43920</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>26</v>
+      <c r="F14" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="10" t="n">
+        <v>43</v>
+      </c>
+      <c r="M14" s="9" t="n">
         <v>43920</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>26</v>
+      <c r="F15" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M15" s="9" t="n">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M15" s="10" t="n">
+      <c r="E16" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M16" s="9" t="n">
         <v>43920</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>26</v>
+      <c r="F17" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="O17" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>26</v>
+      <c r="F18" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
+      </c>
+      <c r="O18" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>26</v>
+      <c r="F19" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>26</v>
+      <c r="F20" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
+      <c r="F21" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13.3</v>
       </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>13.3</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" s="0" t="n">
-        <v>123344</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>123344</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="4" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="J26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L25" s="10" t="n">
+      <c r="K26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L26" s="9" t="n">
         <v>43919</v>
       </c>
-      <c r="M25" s="10" t="n">
+      <c r="M26" s="9" t="n">
         <v>43920</v>
       </c>
-      <c r="N25" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O25" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>27</v>
+      <c r="N26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>26</v>
+      <c r="F27" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>26</v>
+      <c r="F28" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>26</v>
+      <c r="F29" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>26</v>
+      <c r="F30" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>26</v>
+      <c r="F31" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>26</v>
+      <c r="F32" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>26</v>
+      <c r="F33" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>26</v>
+      <c r="F34" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>26</v>
+      <c r="F35" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>26</v>
+      <c r="F36" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>26</v>
+      <c r="F37" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>26</v>
+      <c r="F38" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>26</v>
+      <c r="F39" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F40" s="6" t="s">
-        <v>26</v>
+      <c r="F40" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>86</v>
+        <v>43</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>26</v>
+      <c r="F41" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F42" s="6" t="s">
-        <v>26</v>
+      <c r="F42" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F43" s="6" t="s">
-        <v>26</v>
+      <c r="F43" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>26</v>
+      <c r="F44" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F45" s="6" t="s">
-        <v>26</v>
+      <c r="F45" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>26</v>
+      <c r="F46" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F47" s="6" t="s">
-        <v>26</v>
+      <c r="F47" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F48" s="6" t="s">
-        <v>26</v>
+      <c r="F48" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>27</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="Adactrain@1"/>
-    <hyperlink ref="G4" r:id="rId2" display="Adactrain@1"/>
-    <hyperlink ref="G5" r:id="rId3" display="Adactrain@1"/>
-    <hyperlink ref="G6" r:id="rId4" display="Adactrain@1"/>
-    <hyperlink ref="G7" r:id="rId5" display="Adactrain@1"/>
-    <hyperlink ref="G8" r:id="rId6" display="Adactrain@1"/>
-    <hyperlink ref="G9" r:id="rId7" display="Adactrain@1"/>
-    <hyperlink ref="G10" r:id="rId8" display="Adactrain@1"/>
-    <hyperlink ref="G11" r:id="rId9" display="Adactrain@1"/>
-    <hyperlink ref="G12" r:id="rId10" display="Adactrain@1"/>
-    <hyperlink ref="G13" r:id="rId11" display="Adactrain@1"/>
-    <hyperlink ref="G14" r:id="rId12" display="Adactrain@1"/>
-    <hyperlink ref="G15" r:id="rId13" display="Adactrain@1"/>
-    <hyperlink ref="G16" r:id="rId14" display="Adactrain@1"/>
-    <hyperlink ref="G17" r:id="rId15" display="Adactrain@1"/>
-    <hyperlink ref="G18" r:id="rId16" display="Adactrain@1"/>
-    <hyperlink ref="G19" r:id="rId17" display="Adactrain@1"/>
-    <hyperlink ref="G20" r:id="rId18" display="Adactrain@1"/>
-    <hyperlink ref="G25" r:id="rId19" display="Adactrain@1"/>
-    <hyperlink ref="G26" r:id="rId20" display="Adactrain@1"/>
-    <hyperlink ref="G27" r:id="rId21" display="Adactrain@1"/>
-    <hyperlink ref="G28" r:id="rId22" display="Adactrain@1"/>
-    <hyperlink ref="G29" r:id="rId23" display="Adactrain@1"/>
-    <hyperlink ref="G30" r:id="rId24" display="Adactrain@1"/>
-    <hyperlink ref="G31" r:id="rId25" display="Adactrain@1"/>
-    <hyperlink ref="G32" r:id="rId26" display="Adactrain@1"/>
-    <hyperlink ref="G33" r:id="rId27" display="Adactrain@1"/>
-    <hyperlink ref="G34" r:id="rId28" display="Adactrain@1"/>
-    <hyperlink ref="G35" r:id="rId29" display="Adactrain@1"/>
-    <hyperlink ref="G36" r:id="rId30" display="Adactrain@1"/>
-    <hyperlink ref="G37" r:id="rId31" display="Adactrain@1"/>
-    <hyperlink ref="G38" r:id="rId32" display="Adactrain@1"/>
-    <hyperlink ref="G39" r:id="rId33" display="Adactrain@1"/>
-    <hyperlink ref="G40" r:id="rId34" display="Adactrain@1"/>
-    <hyperlink ref="G41" r:id="rId35" display="Adactrain@1"/>
-    <hyperlink ref="G42" r:id="rId36" display="Adactrain@1"/>
-    <hyperlink ref="G43" r:id="rId37" display="Adactrain@1"/>
-    <hyperlink ref="G44" r:id="rId38" display="Adactrain@1"/>
-    <hyperlink ref="G45" r:id="rId39" display="Adactrain@1"/>
-    <hyperlink ref="G46" r:id="rId40" display="Adactrain@1"/>
-    <hyperlink ref="G47" r:id="rId41" display="Adactrain@1"/>
-    <hyperlink ref="G48" r:id="rId42" display="Adactrain@1"/>
+    <hyperlink ref="G5" r:id="rId1" display="Adactrain@1"/>
+    <hyperlink ref="G6" r:id="rId2" display="Adactrain@1"/>
+    <hyperlink ref="G7" r:id="rId3" display="Adactrain@1"/>
+    <hyperlink ref="G8" r:id="rId4" display="Adactrain@1"/>
+    <hyperlink ref="G9" r:id="rId5" display="Adactrain@1"/>
+    <hyperlink ref="G10" r:id="rId6" display="Adactrain@1"/>
+    <hyperlink ref="G11" r:id="rId7" display="Adactrain@1"/>
+    <hyperlink ref="G12" r:id="rId8" display="Adactrain@1"/>
+    <hyperlink ref="G13" r:id="rId9" display="Adactrain@1"/>
+    <hyperlink ref="G14" r:id="rId10" display="Adactrain@1"/>
+    <hyperlink ref="G15" r:id="rId11" display="Adactrain@1"/>
+    <hyperlink ref="G16" r:id="rId12" display="Adactrain@1"/>
+    <hyperlink ref="G17" r:id="rId13" display="Adactrain@1"/>
+    <hyperlink ref="G18" r:id="rId14" display="Adactrain@1"/>
+    <hyperlink ref="G19" r:id="rId15" display="Adactrain@1"/>
+    <hyperlink ref="G20" r:id="rId16" display="Adactrain@1"/>
+    <hyperlink ref="G21" r:id="rId17" display="Adactrain@1"/>
+    <hyperlink ref="G26" r:id="rId18" display="Adactrain@1"/>
+    <hyperlink ref="G27" r:id="rId19" display="Adactrain@1"/>
+    <hyperlink ref="G28" r:id="rId20" display="Adactrain@1"/>
+    <hyperlink ref="G29" r:id="rId21" display="Adactrain@1"/>
+    <hyperlink ref="G30" r:id="rId22" display="Adactrain@1"/>
+    <hyperlink ref="G31" r:id="rId23" display="Adactrain@1"/>
+    <hyperlink ref="G32" r:id="rId24" display="Adactrain@1"/>
+    <hyperlink ref="G33" r:id="rId25" display="Adactrain@1"/>
+    <hyperlink ref="G34" r:id="rId26" display="Adactrain@1"/>
+    <hyperlink ref="G35" r:id="rId27" display="Adactrain@1"/>
+    <hyperlink ref="G36" r:id="rId28" display="Adactrain@1"/>
+    <hyperlink ref="G37" r:id="rId29" display="Adactrain@1"/>
+    <hyperlink ref="G38" r:id="rId30" display="Adactrain@1"/>
+    <hyperlink ref="G39" r:id="rId31" display="Adactrain@1"/>
+    <hyperlink ref="G40" r:id="rId32" display="Adactrain@1"/>
+    <hyperlink ref="G41" r:id="rId33" display="Adactrain@1"/>
+    <hyperlink ref="G42" r:id="rId34" display="Adactrain@1"/>
+    <hyperlink ref="G43" r:id="rId35" display="Adactrain@1"/>
+    <hyperlink ref="G44" r:id="rId36" display="Adactrain@1"/>
+    <hyperlink ref="G45" r:id="rId37" display="Adactrain@1"/>
+    <hyperlink ref="G46" r:id="rId38" display="Adactrain@1"/>
+    <hyperlink ref="G47" r:id="rId39" display="Adactrain@1"/>
+    <hyperlink ref="G48" r:id="rId40" display="Adactrain@1"/>
+    <hyperlink ref="G49" r:id="rId41" display="Adactrain@1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added java doc comments, finished test case to reset the search criteria. Converted to testng.class ,configured testng.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -204,22 +204,22 @@
     <t xml:space="preserve">User_is_able_to_book_a_hotel</t>
   </si>
   <si>
+    <t xml:space="preserve">testuser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testuser12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billing address of test user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VISA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_view_itinerary</t>
+  </si>
+  <si>
     <t xml:space="preserve">iPhone_SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testuser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testuser12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billing address of test user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VISA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User_is_able_to_view_itinerary</t>
   </si>
   <si>
     <t xml:space="preserve">adactmobtest</t>
@@ -912,14 +912,15 @@
   <dimension ref="A1:AB54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="87.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.08"/>
@@ -1214,7 +1215,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>51</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>13.3</v>
@@ -1261,19 +1262,19 @@
         <v>50</v>
       </c>
       <c r="P8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="R8" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="S8" s="11" t="n">
         <v>1234567891234570</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V8" s="0" t="n">
         <v>1223</v>
@@ -1284,7 +1285,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -1293,7 +1294,7 @@
         <v>30</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>13.3</v>
@@ -1674,7 +1675,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13.3</v>
@@ -1700,7 +1701,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>13.3</v>
@@ -1726,7 +1727,7 @@
         <v>30</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>13.3</v>
@@ -1749,7 +1750,7 @@
         <v>30</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>13.3</v>
@@ -1772,7 +1773,7 @@
         <v>30</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>13.3</v>
@@ -1795,7 +1796,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>13.3</v>
@@ -1814,7 +1815,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>13.3</v>
@@ -1831,7 +1832,7 @@
         <v>30</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>13.3</v>
@@ -1854,7 +1855,7 @@
         <v>30</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>13.3</v>
@@ -1871,7 +1872,7 @@
         <v>30</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13.3</v>
@@ -1918,7 +1919,7 @@
         <v>30</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13.3</v>
@@ -1941,7 +1942,7 @@
         <v>30</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>13.3</v>
@@ -1964,7 +1965,7 @@
         <v>30</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>13.3</v>
@@ -1987,7 +1988,7 @@
         <v>30</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13.3</v>
@@ -2010,7 +2011,7 @@
         <v>30</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13.3</v>
@@ -2033,7 +2034,7 @@
         <v>30</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>13.3</v>
@@ -2056,7 +2057,7 @@
         <v>30</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>13.3</v>
@@ -2079,7 +2080,7 @@
         <v>30</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>13.3</v>
@@ -2102,7 +2103,7 @@
         <v>30</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>13.3</v>
@@ -2125,7 +2126,7 @@
         <v>30</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>13.3</v>
@@ -2148,7 +2149,7 @@
         <v>30</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>13.3</v>
@@ -2171,7 +2172,7 @@
         <v>30</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>13.3</v>
@@ -2194,7 +2195,7 @@
         <v>30</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>13.3</v>
@@ -2220,7 +2221,7 @@
         <v>30</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13.3</v>
@@ -2246,7 +2247,7 @@
         <v>30</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13.3</v>
@@ -2272,7 +2273,7 @@
         <v>30</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13.3</v>
@@ -2295,7 +2296,7 @@
         <v>30</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>13.3</v>
@@ -2321,7 +2322,7 @@
         <v>30</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>13.3</v>
@@ -2344,7 +2345,7 @@
         <v>30</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E50" s="5" t="n">
         <v>13.3</v>
@@ -2367,7 +2368,7 @@
         <v>30</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>13.3</v>
@@ -2390,7 +2391,7 @@
         <v>30</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>13.3</v>
@@ -2413,7 +2414,7 @@
         <v>30</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>13.3</v>
@@ -2436,7 +2437,7 @@
         <v>30</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>13.3</v>

</xml_diff>

<commit_message>
Modified home class and testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="128">
   <si>
     <t xml:space="preserve">Test_Case_Name</t>
   </si>
@@ -154,6 +154,30 @@
     <t xml:space="preserve">User_is_able_to_search_hotel_with_location_and_hotelname</t>
   </si>
   <si>
+    <t xml:space="preserve">testusersbin16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ED337V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_Search_Hotel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sydney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel Creek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 - Two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_reset_the_search_criteria</t>
+  </si>
+  <si>
     <t xml:space="preserve">simulator</t>
   </si>
   <si>
@@ -163,34 +187,16 @@
     <t xml:space="preserve">iPhone SE</t>
   </si>
   <si>
-    <t xml:space="preserve">testusersbin16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ED337V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User_is_able_to_reset_the_search_criteria</t>
-  </si>
-  <si>
     <t xml:space="preserve">testusersbin20</t>
   </si>
   <si>
     <t xml:space="preserve">testpw123)</t>
   </si>
   <si>
-    <t xml:space="preserve">Sydney</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hotel Creek,Hotel Sunshine,Hotel Hervey,Hotel Cornice</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard</t>
-  </si>
-  <si>
     <t xml:space="preserve">User_is_able_to_book_a_hotel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hotel Creek</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_view_itinerary</t>
@@ -822,12 +828,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -927,13 +933,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD56"/>
+  <dimension ref="A1:AD57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="87.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -1187,604 +1193,625 @@
         <v>43</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="G7" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="K8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="10" t="n">
+        <v>43919</v>
+      </c>
+      <c r="M8" s="10" t="n">
+        <v>43920</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" s="0" t="s">
+      <c r="H11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>43919</v>
+      </c>
+      <c r="M12" s="10" t="n">
+        <v>43920</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="R12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="S12" s="12" t="n">
+        <v>1234567891234570</v>
+      </c>
+      <c r="T12" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>1223</v>
+      </c>
+      <c r="W12" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="10" t="n">
+        <v>43975</v>
+      </c>
+      <c r="M13" s="10" t="n">
+        <v>43977</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="R13" s="9"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="13"/>
+      <c r="W13" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="X13" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y13" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC13" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L11" s="11" t="n">
-        <v>43919</v>
-      </c>
-      <c r="M11" s="11" t="n">
-        <v>43920</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="P11" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q11" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="R11" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="S11" s="12" t="n">
-        <v>1234567891234570</v>
-      </c>
-      <c r="T11" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="V11" s="0" t="n">
-        <v>1223</v>
-      </c>
-      <c r="W11" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="11" t="n">
-        <v>43975</v>
-      </c>
-      <c r="M12" s="11" t="n">
-        <v>43977</v>
-      </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="Q12" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="R12" s="9"/>
-      <c r="S12" s="12"/>
-      <c r="T12" s="13"/>
-      <c r="W12" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="X12" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y12" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC12" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="E14" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>77</v>
+    <row r="15" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="s">
         <v>79</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J17" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
+    <row r="18" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
         <v>83</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="K18" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+    <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="11" t="s">
         <v>85</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="L19" s="11" t="n">
-        <v>43919</v>
+        <v>70</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="9" t="s">
-        <v>86</v>
+      <c r="A20" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="L20" s="11" t="n">
+        <v>70</v>
+      </c>
+      <c r="L20" s="10" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="L21" s="11" t="n">
+        <v>70</v>
+      </c>
+      <c r="L21" s="10" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="M22" s="11" t="n">
-        <v>43920</v>
+        <v>70</v>
+      </c>
+      <c r="L22" s="10" t="n">
+        <v>43919</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="M23" s="11" t="n">
+        <v>70</v>
+      </c>
+      <c r="M23" s="10" t="n">
         <v>43920</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="M24" s="11" t="n">
+        <v>70</v>
+      </c>
+      <c r="M24" s="10" t="n">
         <v>43920</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="N25" s="9" t="s">
-        <v>92</v>
+        <v>70</v>
+      </c>
+      <c r="M25" s="10" t="n">
+        <v>43920</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,134 +1819,137 @@
         <v>93</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="O26" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N26" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
         <v>95</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>13.3</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13.3</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="G31" s="0" t="n">
-        <v>123344</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,391 +1957,388 @@
         <v>101</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>123344</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L33" s="11" t="n">
+    </row>
+    <row r="34" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L34" s="10" t="n">
         <v>43919</v>
       </c>
-      <c r="M33" s="11" t="n">
+      <c r="M34" s="10" t="n">
         <v>43920</v>
       </c>
-      <c r="N33" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E34" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>68</v>
+      <c r="N34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,24 +2346,24 @@
         <v>118</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H48" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="H48" s="4" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2345,48 +2372,48 @@
         <v>120</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E50" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>122</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2394,177 +2421,203 @@
         <v>123</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="s">
+        <v>127</v>
+      </c>
       <c r="B55" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E57" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G12" r:id="rId1" display="Adactrain@1"/>
-    <hyperlink ref="G13" r:id="rId2" display="Adactrain@1"/>
-    <hyperlink ref="G14" r:id="rId3" display="Adactrain@1"/>
-    <hyperlink ref="G15" r:id="rId4" display="Adactrain@1"/>
-    <hyperlink ref="G16" r:id="rId5" display="Adactrain@1"/>
-    <hyperlink ref="G17" r:id="rId6" display="Adactrain@1"/>
-    <hyperlink ref="G18" r:id="rId7" display="Adactrain@1"/>
-    <hyperlink ref="G19" r:id="rId8" display="Adactrain@1"/>
-    <hyperlink ref="G20" r:id="rId9" display="Adactrain@1"/>
-    <hyperlink ref="G21" r:id="rId10" display="Adactrain@1"/>
-    <hyperlink ref="G22" r:id="rId11" display="Adactrain@1"/>
-    <hyperlink ref="G23" r:id="rId12" display="Adactrain@1"/>
-    <hyperlink ref="G24" r:id="rId13" display="Adactrain@1"/>
-    <hyperlink ref="G25" r:id="rId14" display="Adactrain@1"/>
-    <hyperlink ref="G26" r:id="rId15" display="Adactrain@1"/>
-    <hyperlink ref="G27" r:id="rId16" display="Adactrain@1"/>
-    <hyperlink ref="G28" r:id="rId17" display="Adactrain@1"/>
-    <hyperlink ref="G29" r:id="rId18" display="Adactrain@1"/>
-    <hyperlink ref="G33" r:id="rId19" display="Adactrain@1"/>
-    <hyperlink ref="G34" r:id="rId20" display="Adactrain@1"/>
-    <hyperlink ref="G35" r:id="rId21" display="Adactrain@1"/>
-    <hyperlink ref="G36" r:id="rId22" display="Adactrain@1"/>
-    <hyperlink ref="G37" r:id="rId23" display="Adactrain@1"/>
-    <hyperlink ref="G38" r:id="rId24" display="Adactrain@1"/>
-    <hyperlink ref="G39" r:id="rId25" display="Adactrain@1"/>
-    <hyperlink ref="G40" r:id="rId26" display="Adactrain@1"/>
-    <hyperlink ref="G41" r:id="rId27" display="Adactrain@1"/>
-    <hyperlink ref="G42" r:id="rId28" display="Adactrain@1"/>
-    <hyperlink ref="G43" r:id="rId29" display="Adactrain@1"/>
-    <hyperlink ref="G44" r:id="rId30" display="Adactrain@1"/>
-    <hyperlink ref="G45" r:id="rId31" display="Adactrain@1"/>
-    <hyperlink ref="G46" r:id="rId32" display="Adactrain@1"/>
-    <hyperlink ref="G47" r:id="rId33" display="Adactrain@1"/>
-    <hyperlink ref="G48" r:id="rId34" display="Adactrain@1"/>
-    <hyperlink ref="G49" r:id="rId35" display="Adactrain@1"/>
-    <hyperlink ref="G50" r:id="rId36" display="Adactrain@1"/>
-    <hyperlink ref="G51" r:id="rId37" display="Adactrain@1"/>
-    <hyperlink ref="G52" r:id="rId38" display="Adactrain@1"/>
-    <hyperlink ref="G53" r:id="rId39" display="Adactrain@1"/>
-    <hyperlink ref="G54" r:id="rId40" display="Adactrain@1"/>
-    <hyperlink ref="G55" r:id="rId41" display="Adactrain@1"/>
-    <hyperlink ref="G56" r:id="rId42" display="Adactrain@1"/>
+    <hyperlink ref="G13" r:id="rId1" display="Adactrain@1"/>
+    <hyperlink ref="G14" r:id="rId2" display="Adactrain@1"/>
+    <hyperlink ref="G15" r:id="rId3" display="Adactrain@1"/>
+    <hyperlink ref="G16" r:id="rId4" display="Adactrain@1"/>
+    <hyperlink ref="G17" r:id="rId5" display="Adactrain@1"/>
+    <hyperlink ref="G18" r:id="rId6" display="Adactrain@1"/>
+    <hyperlink ref="G19" r:id="rId7" display="Adactrain@1"/>
+    <hyperlink ref="G20" r:id="rId8" display="Adactrain@1"/>
+    <hyperlink ref="G21" r:id="rId9" display="Adactrain@1"/>
+    <hyperlink ref="G22" r:id="rId10" display="Adactrain@1"/>
+    <hyperlink ref="G23" r:id="rId11" display="Adactrain@1"/>
+    <hyperlink ref="G24" r:id="rId12" display="Adactrain@1"/>
+    <hyperlink ref="G25" r:id="rId13" display="Adactrain@1"/>
+    <hyperlink ref="G26" r:id="rId14" display="Adactrain@1"/>
+    <hyperlink ref="G27" r:id="rId15" display="Adactrain@1"/>
+    <hyperlink ref="G28" r:id="rId16" display="Adactrain@1"/>
+    <hyperlink ref="G29" r:id="rId17" display="Adactrain@1"/>
+    <hyperlink ref="G30" r:id="rId18" display="Adactrain@1"/>
+    <hyperlink ref="G34" r:id="rId19" display="Adactrain@1"/>
+    <hyperlink ref="G35" r:id="rId20" display="Adactrain@1"/>
+    <hyperlink ref="G36" r:id="rId21" display="Adactrain@1"/>
+    <hyperlink ref="G37" r:id="rId22" display="Adactrain@1"/>
+    <hyperlink ref="G38" r:id="rId23" display="Adactrain@1"/>
+    <hyperlink ref="G39" r:id="rId24" display="Adactrain@1"/>
+    <hyperlink ref="G40" r:id="rId25" display="Adactrain@1"/>
+    <hyperlink ref="G41" r:id="rId26" display="Adactrain@1"/>
+    <hyperlink ref="G42" r:id="rId27" display="Adactrain@1"/>
+    <hyperlink ref="G43" r:id="rId28" display="Adactrain@1"/>
+    <hyperlink ref="G44" r:id="rId29" display="Adactrain@1"/>
+    <hyperlink ref="G45" r:id="rId30" display="Adactrain@1"/>
+    <hyperlink ref="G46" r:id="rId31" display="Adactrain@1"/>
+    <hyperlink ref="G47" r:id="rId32" display="Adactrain@1"/>
+    <hyperlink ref="G48" r:id="rId33" display="Adactrain@1"/>
+    <hyperlink ref="G49" r:id="rId34" display="Adactrain@1"/>
+    <hyperlink ref="G50" r:id="rId35" display="Adactrain@1"/>
+    <hyperlink ref="G51" r:id="rId36" display="Adactrain@1"/>
+    <hyperlink ref="G52" r:id="rId37" display="Adactrain@1"/>
+    <hyperlink ref="G53" r:id="rId38" display="Adactrain@1"/>
+    <hyperlink ref="G54" r:id="rId39" display="Adactrain@1"/>
+    <hyperlink ref="G55" r:id="rId40" display="Adactrain@1"/>
+    <hyperlink ref="G56" r:id="rId41" display="Adactrain@1"/>
+    <hyperlink ref="G57" r:id="rId42" display="Adactrain@1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Committing select hotel and home page changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="130">
   <si>
     <t xml:space="preserve">Test_Case_Name</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Location</t>
   </si>
   <si>
+    <t xml:space="preserve">Hotel List</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hotels</t>
   </si>
   <si>
@@ -151,6 +154,9 @@
     <t xml:space="preserve">User_is_able_to_Search_Hotel_with_Location</t>
   </si>
   <si>
+    <t xml:space="preserve">Hotel Creek,Hotel Sunshine,Hotel Hervey,Hotel Cornice</t>
+  </si>
+  <si>
     <t xml:space="preserve">User_is_able_to_search_hotel_with_location_and_hotelname</t>
   </si>
   <si>
@@ -160,15 +166,18 @@
     <t xml:space="preserve">ED337V</t>
   </si>
   <si>
+    <t xml:space="preserve">Hotel Creek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel Creek,Hotel Creek,Hotel Creek,Hotel Creek</t>
+  </si>
+  <si>
     <t xml:space="preserve">User_is_able_to_Search_Hotel</t>
   </si>
   <si>
     <t xml:space="preserve">Sydney</t>
   </si>
   <si>
-    <t xml:space="preserve">Hotel Creek</t>
-  </si>
-  <si>
     <t xml:space="preserve">Standard</t>
   </si>
   <si>
@@ -191,9 +200,6 @@
   </si>
   <si>
     <t xml:space="preserve">testpw123)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hotel Creek,Hotel Sunshine,Hotel Hervey,Hotel Cornice</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_book_a_hotel</t>
@@ -682,7 +688,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="0000000000000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -731,6 +737,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -787,7 +798,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -828,6 +839,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -852,7 +867,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -933,13 +948,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD57"/>
+  <dimension ref="A1:AE57"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="87.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -949,21 +964,22 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="17.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="24.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="0" width="27.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="19.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="24.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="27.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="19.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1048,7 +1064,7 @@
       <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
       <c r="AC1" s="2" t="s">
@@ -1057,896 +1073,918 @@
       <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="AB3" s="9" t="s">
-        <v>38</v>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
+      <c r="AC3" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="AC4" s="0" t="s">
-        <v>40</v>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="AD4" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="47.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="AC6" s="9"/>
+    </row>
+    <row r="7" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-      <c r="AB6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="E7" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>48</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="11" t="n">
         <v>43919</v>
       </c>
-      <c r="M8" s="10" t="n">
+      <c r="N8" s="11" t="n">
         <v>43920</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="O8" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="J9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>49</v>
+      <c r="K10" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>61</v>
+      <c r="L11" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
-        <v>62</v>
+      <c r="A12" s="12" t="s">
+        <v>64</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="K12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" s="10" t="n">
+        <v>52</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="11" t="n">
         <v>43919</v>
       </c>
-      <c r="M12" s="10" t="n">
+      <c r="N12" s="11" t="n">
         <v>43920</v>
       </c>
-      <c r="N12" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="O12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="P12" s="0" t="s">
         <v>63</v>
       </c>
+      <c r="P12" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="Q12" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="R12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="S12" s="12" t="n">
+      <c r="R12" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="T12" s="13" t="n">
         <v>1234567891234570</v>
       </c>
-      <c r="T12" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="V12" s="0" t="n">
+      <c r="U12" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="W12" s="0" t="n">
         <v>1223</v>
       </c>
-      <c r="W12" s="4" t="n">
+      <c r="X12" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>67</v>
+      <c r="A13" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K13" s="15" t="n">
+      <c r="L13" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="10" t="n">
+      <c r="M13" s="11" t="n">
         <v>43975</v>
       </c>
-      <c r="M13" s="10" t="n">
+      <c r="N13" s="11" t="n">
         <v>43977</v>
       </c>
-      <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="5" t="n">
+      <c r="P13" s="4"/>
+      <c r="Q13" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="Q13" s="5" t="n">
+      <c r="R13" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="R13" s="9"/>
-      <c r="S13" s="12"/>
+      <c r="S13" s="9"/>
       <c r="T13" s="13"/>
-      <c r="W13" s="15" t="n">
+      <c r="U13" s="14"/>
+      <c r="X13" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="X13" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y13" s="5" t="n">
+      <c r="Y13" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z13" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="Z13" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="AA13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC13" s="0" t="s">
         <v>76</v>
       </c>
+      <c r="AB13" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD13" s="0" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
-        <v>77</v>
+      <c r="A14" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>69</v>
+      <c r="F14" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>78</v>
+      <c r="A15" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>69</v>
+      <c r="F15" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
-        <v>79</v>
+      <c r="A16" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>69</v>
+      <c r="F16" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>80</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>81</v>
+      <c r="A17" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>69</v>
+      <c r="F17" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H17" s="7"/>
-      <c r="I17" s="1" t="s">
-        <v>82</v>
+      <c r="I17" s="7"/>
+      <c r="J17" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
-        <v>83</v>
+      <c r="A18" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>69</v>
+      <c r="F18" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>84</v>
+        <v>72</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
-        <v>85</v>
+      <c r="A19" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>69</v>
+      <c r="F19" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>86</v>
+        <v>72</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
-        <v>87</v>
+      <c r="A20" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>69</v>
+      <c r="F20" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="M20" s="11" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>69</v>
+      <c r="F21" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L21" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="M21" s="11" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>69</v>
+      <c r="F22" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L22" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="M22" s="11" t="n">
         <v>43919</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>69</v>
+      <c r="F23" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="M23" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="N23" s="11" t="n">
         <v>43920</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F24" s="14" t="s">
-        <v>69</v>
+      <c r="F24" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="M24" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="N24" s="11" t="n">
         <v>43920</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>69</v>
+      <c r="F25" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="M25" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="N25" s="11" t="n">
         <v>43920</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>69</v>
+      <c r="F26" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="N26" s="9" t="s">
-        <v>94</v>
+        <v>72</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F27" s="14" t="s">
-        <v>69</v>
+      <c r="F27" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="O27" s="9" t="s">
-        <v>96</v>
+        <v>72</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F28" s="14" t="s">
-        <v>69</v>
+      <c r="F28" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>69</v>
+      <c r="F29" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F30" s="14" t="s">
-        <v>69</v>
+      <c r="F30" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13.3</v>
@@ -1954,22 +1992,22 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G32" s="0" t="n">
         <v>123344</v>
@@ -1977,16 +2015,16 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>13.3</v>
@@ -1994,584 +2032,587 @@
     </row>
     <row r="34" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K34" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L34" s="10" t="n">
+      <c r="L34" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M34" s="11" t="n">
         <v>43919</v>
       </c>
-      <c r="M34" s="10" t="n">
+      <c r="N34" s="11" t="n">
         <v>43920</v>
       </c>
-      <c r="N34" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="O34" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F35" s="14" t="s">
-        <v>69</v>
+      <c r="F35" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F36" s="14" t="s">
-        <v>69</v>
+      <c r="F36" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F37" s="14" t="s">
-        <v>69</v>
+      <c r="F37" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F38" s="14" t="s">
-        <v>69</v>
+      <c r="F38" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F39" s="14" t="s">
-        <v>69</v>
+      <c r="F39" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F40" s="14" t="s">
-        <v>69</v>
+      <c r="F40" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F41" s="14" t="s">
-        <v>69</v>
+      <c r="F41" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F42" s="14" t="s">
-        <v>69</v>
+      <c r="F42" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F43" s="14" t="s">
-        <v>69</v>
+      <c r="F43" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F44" s="14" t="s">
-        <v>69</v>
+      <c r="F44" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F45" s="14" t="s">
-        <v>69</v>
+      <c r="F45" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F46" s="14" t="s">
-        <v>69</v>
+      <c r="F46" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F47" s="14" t="s">
-        <v>69</v>
+      <c r="F47" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>71</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="I47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F48" s="14" t="s">
-        <v>69</v>
+      <c r="F48" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>119</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="I48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F49" s="14" t="s">
-        <v>69</v>
+      <c r="F49" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E50" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F50" s="14" t="s">
-        <v>69</v>
+      <c r="F50" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F51" s="14" t="s">
-        <v>69</v>
+      <c r="F51" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>124</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="I51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F52" s="14" t="s">
-        <v>69</v>
+      <c r="F52" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F53" s="14" t="s">
-        <v>69</v>
+      <c r="F53" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F54" s="14" t="s">
-        <v>69</v>
+      <c r="F54" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F55" s="14" t="s">
-        <v>69</v>
+      <c r="F55" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F56" s="14" t="s">
-        <v>69</v>
+      <c r="F56" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F57" s="14" t="s">
-        <v>69</v>
+      <c r="F57" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing selected hotel details class and test scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="128">
   <si>
     <t xml:space="preserve">Test_Case_Name</t>
   </si>
@@ -172,21 +172,53 @@
     <t xml:space="preserve">Hotel Creek</t>
   </si>
   <si>
+    <t xml:space="preserve">User_is_able_to_select_hotel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotel Hervey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> One</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">User_is_able_to_Search_Hotel</t>
   </si>
   <si>
-    <t xml:space="preserve">Standard</t>
-  </si>
-  <si>
     <t xml:space="preserve">2 - Two</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_reset_the_search_criteria</t>
   </si>
   <si>
-    <t xml:space="preserve">Hotel Hervey</t>
-  </si>
-  <si>
     <t xml:space="preserve">User_is_able_to_book_a_hotel</t>
   </si>
   <si>
@@ -206,35 +238,6 @@
   </si>
   <si>
     <t xml:space="preserve">ED337V</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> One</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">User_is_shown_an_error_message_when_any_mandatory_field_is_not_entered_and_he_clicks_on_the_search_button</t>
@@ -825,6 +828,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -842,10 +849,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -930,13 +933,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE57"/>
+  <dimension ref="A1:AE58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q9" activeCellId="0" sqref="Q9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="87.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -1230,7 +1233,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>50</v>
       </c>
@@ -1253,36 +1256,36 @@
         <v>35</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="M8" s="10" t="n">
-        <v>43919</v>
-      </c>
-      <c r="N8" s="10" t="n">
-        <v>43920</v>
+      <c r="L8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" s="11" t="n">
+        <v>44026</v>
+      </c>
+      <c r="N8" s="11" t="n">
+        <v>44027</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>32</v>
@@ -1305,25 +1308,34 @@
       <c r="H9" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="I9" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="J9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="M9" s="11" t="n">
+        <v>43919</v>
+      </c>
+      <c r="N9" s="11" t="n">
+        <v>43920</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>32</v>
@@ -1347,33 +1359,42 @@
         <v>44</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>13.3</v>
+        <v>10</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>44</v>
@@ -1381,40 +1402,31 @@
       <c r="J11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L11" s="4" t="s">
+      <c r="K11" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="O11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+      <c r="G12" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>44</v>
@@ -1423,323 +1435,338 @@
         <v>49</v>
       </c>
       <c r="K12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" s="11" t="n">
+        <v>43919</v>
+      </c>
+      <c r="N13" s="11" t="n">
+        <v>43920</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="S13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="T13" s="13" t="n">
+        <v>1234567891234570</v>
+      </c>
+      <c r="U13" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>1223</v>
+      </c>
+      <c r="X13" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M12" s="10" t="n">
-        <v>43919</v>
-      </c>
-      <c r="N12" s="10" t="n">
-        <v>43920</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q12" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="R12" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="S12" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="T12" s="12" t="n">
-        <v>1234567891234570</v>
-      </c>
-      <c r="U12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="W12" s="0" t="n">
-        <v>1223</v>
-      </c>
-      <c r="X12" s="4" t="n">
+      <c r="K14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="10" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="15" t="n">
+      <c r="M14" s="11" t="n">
+        <v>43975</v>
+      </c>
+      <c r="N14" s="11" t="n">
+        <v>43977</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="R14" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S14" s="9"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="14"/>
+      <c r="X14" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="M13" s="10" t="n">
-        <v>43975</v>
-      </c>
-      <c r="N13" s="10" t="n">
-        <v>43977</v>
-      </c>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="R13" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="S13" s="9"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="13"/>
-      <c r="X13" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z13" s="5" t="n">
+      <c r="Y14" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z14" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="AA13" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB13" s="5" t="s">
+      <c r="AA14" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AD13" s="0" t="s">
+      <c r="AB14" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
+      <c r="AD14" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
         <v>77</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>70</v>
+      <c r="F15" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+    <row r="16" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>70</v>
+      <c r="F16" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
+      <c r="B17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="1" t="s">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="B18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K18" s="9" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
+      <c r="B19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K19" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="L19" s="16" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
+      <c r="B20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L20" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M20" s="10" t="n">
-        <v>43919</v>
-      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="12" t="s">
         <v>87</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>70</v>
+      <c r="F21" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="M21" s="11" t="n">
         <v>43919</v>
       </c>
     </row>
@@ -1748,24 +1775,24 @@
         <v>88</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>70</v>
+      <c r="F22" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="M22" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="M22" s="11" t="n">
         <v>43919</v>
       </c>
     </row>
@@ -1774,25 +1801,25 @@
         <v>89</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>70</v>
+      <c r="F23" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="N23" s="10" t="n">
-        <v>43920</v>
+        <v>72</v>
+      </c>
+      <c r="M23" s="11" t="n">
+        <v>43919</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1800,24 +1827,24 @@
         <v>90</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F24" s="14" t="s">
-        <v>70</v>
+      <c r="F24" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="N24" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="N24" s="11" t="n">
         <v>43920</v>
       </c>
     </row>
@@ -1826,100 +1853,103 @@
         <v>91</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>70</v>
+      <c r="F25" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="N25" s="10" t="n">
+        <v>72</v>
+      </c>
+      <c r="N25" s="11" t="n">
         <v>43920</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
         <v>92</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>70</v>
+      <c r="F26" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="O26" s="9" t="s">
-        <v>93</v>
+        <v>72</v>
+      </c>
+      <c r="N26" s="11" t="n">
+        <v>43920</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O27" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="P27" s="9" t="s">
+    </row>
+    <row r="28" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="P28" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1927,22 +1957,22 @@
         <v>97</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E29" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>70</v>
+      <c r="F29" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,22 +1980,22 @@
         <v>98</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F30" s="14" t="s">
-        <v>70</v>
+      <c r="F30" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,16 +2003,22 @@
         <v>99</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13.3</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,109 +2026,103 @@
         <v>100</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13.3</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" s="0" t="n">
-        <v>123344</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" s="5" t="n">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="0" t="n">
+        <v>123344</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="M34" s="10" t="n">
-        <v>43919</v>
-      </c>
-      <c r="N34" s="10" t="n">
-        <v>43920</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P34" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="35" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F35" s="14" t="s">
-        <v>70</v>
+      <c r="F35" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M35" s="11" t="n">
+        <v>43919</v>
+      </c>
+      <c r="N35" s="11" t="n">
+        <v>43920</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2100,22 +2130,22 @@
         <v>105</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F36" s="14" t="s">
-        <v>70</v>
+      <c r="F36" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,22 +2153,22 @@
         <v>106</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F37" s="14" t="s">
-        <v>70</v>
+      <c r="F37" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,22 +2176,22 @@
         <v>107</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F38" s="14" t="s">
-        <v>70</v>
+      <c r="F38" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,22 +2199,22 @@
         <v>108</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F39" s="14" t="s">
-        <v>70</v>
+      <c r="F39" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,68 +2222,68 @@
         <v>109</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F40" s="14" t="s">
-        <v>70</v>
+      <c r="F40" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F41" s="14" t="s">
-        <v>70</v>
+      <c r="F41" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F42" s="14" t="s">
-        <v>70</v>
+      <c r="F42" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2261,22 +2291,22 @@
         <v>112</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F43" s="14" t="s">
-        <v>70</v>
+      <c r="F43" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2284,22 +2314,22 @@
         <v>113</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F44" s="14" t="s">
-        <v>70</v>
+      <c r="F44" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2307,22 +2337,22 @@
         <v>114</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F45" s="14" t="s">
-        <v>70</v>
+      <c r="F45" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,22 +2360,22 @@
         <v>115</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F46" s="14" t="s">
-        <v>70</v>
+      <c r="F46" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,102 +2383,102 @@
         <v>116</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F47" s="14" t="s">
-        <v>70</v>
+      <c r="F47" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I47" s="4"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
         <v>117</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F48" s="14" t="s">
-        <v>70</v>
+      <c r="F48" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="I48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H49" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H49" s="0" t="s">
-        <v>120</v>
-      </c>
+      <c r="I49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H50" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E50" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G50" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2456,95 +2486,95 @@
         <v>122</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F51" s="14" t="s">
-        <v>70</v>
+      <c r="F51" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I51" s="4"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H52" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E52" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G52" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="I52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F53" s="14" t="s">
-        <v>70</v>
+      <c r="F53" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F54" s="14" t="s">
-        <v>70</v>
+      <c r="F54" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2552,108 +2582,131 @@
         <v>126</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F55" s="14" t="s">
-        <v>70</v>
+      <c r="F55" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="9" t="s">
+        <v>127</v>
+      </c>
       <c r="B56" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F56" s="14" t="s">
-        <v>70</v>
+      <c r="F56" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F57" s="14" t="s">
-        <v>70</v>
+      <c r="F57" s="15" t="s">
+        <v>71</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E58" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G13" r:id="rId1" display="Adactrain@1"/>
-    <hyperlink ref="G14" r:id="rId2" display="Adactrain@1"/>
-    <hyperlink ref="G15" r:id="rId3" display="Adactrain@1"/>
-    <hyperlink ref="G16" r:id="rId4" display="Adactrain@1"/>
-    <hyperlink ref="G17" r:id="rId5" display="Adactrain@1"/>
-    <hyperlink ref="G18" r:id="rId6" display="Adactrain@1"/>
-    <hyperlink ref="G19" r:id="rId7" display="Adactrain@1"/>
-    <hyperlink ref="G20" r:id="rId8" display="Adactrain@1"/>
-    <hyperlink ref="G21" r:id="rId9" display="Adactrain@1"/>
-    <hyperlink ref="G22" r:id="rId10" display="Adactrain@1"/>
-    <hyperlink ref="G23" r:id="rId11" display="Adactrain@1"/>
-    <hyperlink ref="G24" r:id="rId12" display="Adactrain@1"/>
-    <hyperlink ref="G25" r:id="rId13" display="Adactrain@1"/>
-    <hyperlink ref="G26" r:id="rId14" display="Adactrain@1"/>
-    <hyperlink ref="G27" r:id="rId15" display="Adactrain@1"/>
-    <hyperlink ref="G28" r:id="rId16" display="Adactrain@1"/>
-    <hyperlink ref="G29" r:id="rId17" display="Adactrain@1"/>
-    <hyperlink ref="G30" r:id="rId18" display="Adactrain@1"/>
-    <hyperlink ref="G34" r:id="rId19" display="Adactrain@1"/>
-    <hyperlink ref="G35" r:id="rId20" display="Adactrain@1"/>
-    <hyperlink ref="G36" r:id="rId21" display="Adactrain@1"/>
-    <hyperlink ref="G37" r:id="rId22" display="Adactrain@1"/>
-    <hyperlink ref="G38" r:id="rId23" display="Adactrain@1"/>
-    <hyperlink ref="G39" r:id="rId24" display="Adactrain@1"/>
-    <hyperlink ref="G40" r:id="rId25" display="Adactrain@1"/>
-    <hyperlink ref="G41" r:id="rId26" display="Adactrain@1"/>
-    <hyperlink ref="G42" r:id="rId27" display="Adactrain@1"/>
-    <hyperlink ref="G43" r:id="rId28" display="Adactrain@1"/>
-    <hyperlink ref="G44" r:id="rId29" display="Adactrain@1"/>
-    <hyperlink ref="G45" r:id="rId30" display="Adactrain@1"/>
-    <hyperlink ref="G46" r:id="rId31" display="Adactrain@1"/>
-    <hyperlink ref="G47" r:id="rId32" display="Adactrain@1"/>
-    <hyperlink ref="G48" r:id="rId33" display="Adactrain@1"/>
-    <hyperlink ref="G49" r:id="rId34" display="Adactrain@1"/>
-    <hyperlink ref="G50" r:id="rId35" display="Adactrain@1"/>
-    <hyperlink ref="G51" r:id="rId36" display="Adactrain@1"/>
-    <hyperlink ref="G52" r:id="rId37" display="Adactrain@1"/>
-    <hyperlink ref="G53" r:id="rId38" display="Adactrain@1"/>
-    <hyperlink ref="G54" r:id="rId39" display="Adactrain@1"/>
-    <hyperlink ref="G55" r:id="rId40" display="Adactrain@1"/>
-    <hyperlink ref="G56" r:id="rId41" display="Adactrain@1"/>
-    <hyperlink ref="G57" r:id="rId42" display="Adactrain@1"/>
+    <hyperlink ref="G14" r:id="rId1" display="Adactrain@1"/>
+    <hyperlink ref="G15" r:id="rId2" display="Adactrain@1"/>
+    <hyperlink ref="G16" r:id="rId3" display="Adactrain@1"/>
+    <hyperlink ref="G17" r:id="rId4" display="Adactrain@1"/>
+    <hyperlink ref="G18" r:id="rId5" display="Adactrain@1"/>
+    <hyperlink ref="G19" r:id="rId6" display="Adactrain@1"/>
+    <hyperlink ref="G20" r:id="rId7" display="Adactrain@1"/>
+    <hyperlink ref="G21" r:id="rId8" display="Adactrain@1"/>
+    <hyperlink ref="G22" r:id="rId9" display="Adactrain@1"/>
+    <hyperlink ref="G23" r:id="rId10" display="Adactrain@1"/>
+    <hyperlink ref="G24" r:id="rId11" display="Adactrain@1"/>
+    <hyperlink ref="G25" r:id="rId12" display="Adactrain@1"/>
+    <hyperlink ref="G26" r:id="rId13" display="Adactrain@1"/>
+    <hyperlink ref="G27" r:id="rId14" display="Adactrain@1"/>
+    <hyperlink ref="G28" r:id="rId15" display="Adactrain@1"/>
+    <hyperlink ref="G29" r:id="rId16" display="Adactrain@1"/>
+    <hyperlink ref="G30" r:id="rId17" display="Adactrain@1"/>
+    <hyperlink ref="G31" r:id="rId18" display="Adactrain@1"/>
+    <hyperlink ref="G35" r:id="rId19" display="Adactrain@1"/>
+    <hyperlink ref="G36" r:id="rId20" display="Adactrain@1"/>
+    <hyperlink ref="G37" r:id="rId21" display="Adactrain@1"/>
+    <hyperlink ref="G38" r:id="rId22" display="Adactrain@1"/>
+    <hyperlink ref="G39" r:id="rId23" display="Adactrain@1"/>
+    <hyperlink ref="G40" r:id="rId24" display="Adactrain@1"/>
+    <hyperlink ref="G41" r:id="rId25" display="Adactrain@1"/>
+    <hyperlink ref="G42" r:id="rId26" display="Adactrain@1"/>
+    <hyperlink ref="G43" r:id="rId27" display="Adactrain@1"/>
+    <hyperlink ref="G44" r:id="rId28" display="Adactrain@1"/>
+    <hyperlink ref="G45" r:id="rId29" display="Adactrain@1"/>
+    <hyperlink ref="G46" r:id="rId30" display="Adactrain@1"/>
+    <hyperlink ref="G47" r:id="rId31" display="Adactrain@1"/>
+    <hyperlink ref="G48" r:id="rId32" display="Adactrain@1"/>
+    <hyperlink ref="G49" r:id="rId33" display="Adactrain@1"/>
+    <hyperlink ref="G50" r:id="rId34" display="Adactrain@1"/>
+    <hyperlink ref="G51" r:id="rId35" display="Adactrain@1"/>
+    <hyperlink ref="G52" r:id="rId36" display="Adactrain@1"/>
+    <hyperlink ref="G53" r:id="rId37" display="Adactrain@1"/>
+    <hyperlink ref="G54" r:id="rId38" display="Adactrain@1"/>
+    <hyperlink ref="G55" r:id="rId39" display="Adactrain@1"/>
+    <hyperlink ref="G56" r:id="rId40" display="Adactrain@1"/>
+    <hyperlink ref="G57" r:id="rId41" display="Adactrain@1"/>
+    <hyperlink ref="G58" r:id="rId42" display="Adactrain@1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Committing and pushing modified changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="131">
   <si>
     <t xml:space="preserve">Test_Case_Name</t>
   </si>
@@ -151,6 +151,9 @@
     <t xml:space="preserve">User_is_able_to_logout</t>
   </si>
   <si>
+    <t xml:space="preserve">User_is_able_to_cancel_a_hotel_booking</t>
+  </si>
+  <si>
     <t xml:space="preserve">User_is_able_to_Search_Hotel_with_Location</t>
   </si>
   <si>
@@ -225,61 +228,67 @@
     <t xml:space="preserve">User_is_able_to_view_itinerary</t>
   </si>
   <si>
+    <t xml:space="preserve">testuser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testuser12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">650MP69010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUD $100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUD $121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_view_booked_hotel_details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_shown_an_error_message_when_any_mandatory_field_is_not_entered_and_he_clicks_on_the_search_button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billing address of test user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VISA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_scroll_down_and_up_on_the_search_hotel_screen</t>
+  </si>
+  <si>
     <t xml:space="preserve">simulator</t>
   </si>
   <si>
     <t xml:space="preserve">iOS</t>
   </si>
   <si>
+    <t xml:space="preserve">iPhone_SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adactmobtest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adactrain@1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">562C514569</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUD $150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUD $341</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_view_the_drop_down_list_in_locations</t>
+  </si>
+  <si>
     <t xml:space="preserve">iPhone SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testusersbin2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ED337V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User_is_shown_an_error_message_when_any_mandatory_field_is_not_entered_and_he_clicks_on_the_search_button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testuser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testuser12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billing address of test user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VISA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User_is_able_to_scroll_down_and_up_on_the_search_hotel_screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iPhone_SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adactmobtest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adactrain@1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">562C514569</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUD $150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUD $341</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User_is_able_to_view_the_drop_down_list_in_locations</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_view_list_of_hotels_in_the_drop_down_menu_</t>
@@ -933,13 +942,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE58"/>
+  <dimension ref="A1:AE60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X6" activeCellId="0" sqref="X6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="87.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -1170,7 +1179,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="47.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
@@ -1192,18 +1201,16 @@
       <c r="G6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="8"/>
+      <c r="X6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="47.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="8"/>
-      <c r="AC6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>32</v>
@@ -1223,19 +1230,18 @@
       <c r="G7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>47</v>
+      <c r="H7" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>49</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="J7" s="8"/>
+      <c r="AC7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>32</v>
@@ -1256,36 +1262,18 @@
         <v>35</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" s="11" t="n">
-        <v>44026</v>
-      </c>
-      <c r="N8" s="11" t="n">
-        <v>44027</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>32</v>
@@ -1306,36 +1294,36 @@
         <v>35</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="L9" s="10" t="n">
+        <v>1</v>
       </c>
       <c r="M9" s="11" t="n">
-        <v>43919</v>
+        <v>44026</v>
       </c>
       <c r="N9" s="11" t="n">
-        <v>43920</v>
+        <v>44027</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>32</v>
@@ -1356,22 +1344,31 @@
         <v>35</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="M10" s="11" t="n">
+        <v>43919</v>
+      </c>
+      <c r="N10" s="11" t="n">
+        <v>43920</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,59 +1394,59 @@
         <v>35</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>53</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
-        <v>64</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>32</v>
@@ -1470,353 +1467,434 @@
         <v>35</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" s="4" t="s">
         <v>53</v>
       </c>
+      <c r="L13" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="M13" s="11" t="n">
-        <v>43919</v>
+        <v>44007</v>
       </c>
       <c r="N13" s="11" t="n">
-        <v>43920</v>
+        <v>44008</v>
       </c>
       <c r="O13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q13" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="R13" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB13" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q13" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="R13" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="S13" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="T13" s="13" t="n">
-        <v>1234567891234570</v>
-      </c>
-      <c r="U13" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="W13" s="0" t="n">
-        <v>1223</v>
-      </c>
-      <c r="X13" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="L14" s="10" t="n">
         <v>1</v>
       </c>
       <c r="M14" s="11" t="n">
+        <v>44007</v>
+      </c>
+      <c r="N14" s="11" t="n">
+        <v>44008</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q14" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="X14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB14" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M15" s="11" t="n">
+        <v>43919</v>
+      </c>
+      <c r="N15" s="11" t="n">
+        <v>43920</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="S15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="T15" s="13" t="n">
+        <v>1234567891234570</v>
+      </c>
+      <c r="U15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>1223</v>
+      </c>
+      <c r="X15" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="11" t="n">
         <v>43975</v>
       </c>
-      <c r="N14" s="11" t="n">
+      <c r="N16" s="11" t="n">
         <v>43977</v>
       </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="5" t="n">
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="R14" s="5" t="n">
+      <c r="R16" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="S14" s="9"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="14"/>
-      <c r="X14" s="10" t="n">
+      <c r="S16" s="9"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="14"/>
+      <c r="X16" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="Y14" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z14" s="5" t="n">
+      <c r="Y16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z16" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="AA14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AB14" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD14" s="0" t="s">
+      <c r="AA16" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
+      <c r="AB16" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="AD16" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
         <v>79</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E17" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
         <v>81</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E18" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="B19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="K19" s="9" t="s">
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+      <c r="B20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="L20" s="16" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="12" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="B21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K21" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="M21" s="11" t="n">
-        <v>43919</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="12" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="M22" s="11" t="n">
-        <v>43919</v>
+        <v>74</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
-        <v>89</v>
+      <c r="A23" s="12" t="s">
+        <v>90</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="M23" s="11" t="n">
         <v>43919</v>
@@ -1824,241 +1902,253 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="N24" s="11" t="n">
-        <v>43920</v>
+        <v>74</v>
+      </c>
+      <c r="M24" s="11" t="n">
+        <v>43919</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E25" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="N25" s="11" t="n">
-        <v>43920</v>
+        <v>74</v>
+      </c>
+      <c r="M25" s="11" t="n">
+        <v>43919</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="E26" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N26" s="11" t="n">
         <v>43920</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E27" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="O27" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+      <c r="N27" s="11" t="n">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
         <v>95</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E28" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="P28" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N28" s="11" t="n">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
+      <c r="B29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="O29" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
         <v>98</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E30" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="P30" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E31" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13.3</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="G33" s="0" t="n">
-        <v>123344</v>
+      <c r="F33" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,647 +2156,687 @@
         <v>103</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>13.3</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F35" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M35" s="11" t="n">
-        <v>43919</v>
-      </c>
-      <c r="N35" s="11" t="n">
-        <v>43920</v>
-      </c>
-      <c r="O35" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P35" s="4" t="s">
-        <v>53</v>
+      <c r="F35" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <v>123344</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F36" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="37" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E37" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M37" s="11" t="n">
+        <v>43919</v>
+      </c>
+      <c r="N37" s="11" t="n">
+        <v>43920</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E38" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E39" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E40" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F47" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I48" s="4"/>
+        <v>74</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H49" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="I49" s="4"/>
+        <v>74</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
         <v>120</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E50" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H50" s="0" t="s">
-        <v>121</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H51" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E51" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="I51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
         <v>123</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H52" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H52" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="I52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
         <v>125</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>72</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="B57" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="B58" s="4" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>13.3</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E59" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E60" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G60" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G14" r:id="rId1" display="Adactrain@1"/>
-    <hyperlink ref="G15" r:id="rId2" display="Adactrain@1"/>
-    <hyperlink ref="G16" r:id="rId3" display="Adactrain@1"/>
-    <hyperlink ref="G17" r:id="rId4" display="Adactrain@1"/>
-    <hyperlink ref="G18" r:id="rId5" display="Adactrain@1"/>
-    <hyperlink ref="G19" r:id="rId6" display="Adactrain@1"/>
-    <hyperlink ref="G20" r:id="rId7" display="Adactrain@1"/>
-    <hyperlink ref="G21" r:id="rId8" display="Adactrain@1"/>
-    <hyperlink ref="G22" r:id="rId9" display="Adactrain@1"/>
-    <hyperlink ref="G23" r:id="rId10" display="Adactrain@1"/>
-    <hyperlink ref="G24" r:id="rId11" display="Adactrain@1"/>
-    <hyperlink ref="G25" r:id="rId12" display="Adactrain@1"/>
-    <hyperlink ref="G26" r:id="rId13" display="Adactrain@1"/>
-    <hyperlink ref="G27" r:id="rId14" display="Adactrain@1"/>
-    <hyperlink ref="G28" r:id="rId15" display="Adactrain@1"/>
-    <hyperlink ref="G29" r:id="rId16" display="Adactrain@1"/>
-    <hyperlink ref="G30" r:id="rId17" display="Adactrain@1"/>
-    <hyperlink ref="G31" r:id="rId18" display="Adactrain@1"/>
-    <hyperlink ref="G35" r:id="rId19" display="Adactrain@1"/>
-    <hyperlink ref="G36" r:id="rId20" display="Adactrain@1"/>
-    <hyperlink ref="G37" r:id="rId21" display="Adactrain@1"/>
-    <hyperlink ref="G38" r:id="rId22" display="Adactrain@1"/>
-    <hyperlink ref="G39" r:id="rId23" display="Adactrain@1"/>
-    <hyperlink ref="G40" r:id="rId24" display="Adactrain@1"/>
-    <hyperlink ref="G41" r:id="rId25" display="Adactrain@1"/>
-    <hyperlink ref="G42" r:id="rId26" display="Adactrain@1"/>
-    <hyperlink ref="G43" r:id="rId27" display="Adactrain@1"/>
-    <hyperlink ref="G44" r:id="rId28" display="Adactrain@1"/>
-    <hyperlink ref="G45" r:id="rId29" display="Adactrain@1"/>
-    <hyperlink ref="G46" r:id="rId30" display="Adactrain@1"/>
-    <hyperlink ref="G47" r:id="rId31" display="Adactrain@1"/>
-    <hyperlink ref="G48" r:id="rId32" display="Adactrain@1"/>
-    <hyperlink ref="G49" r:id="rId33" display="Adactrain@1"/>
-    <hyperlink ref="G50" r:id="rId34" display="Adactrain@1"/>
-    <hyperlink ref="G51" r:id="rId35" display="Adactrain@1"/>
-    <hyperlink ref="G52" r:id="rId36" display="Adactrain@1"/>
-    <hyperlink ref="G53" r:id="rId37" display="Adactrain@1"/>
-    <hyperlink ref="G54" r:id="rId38" display="Adactrain@1"/>
-    <hyperlink ref="G55" r:id="rId39" display="Adactrain@1"/>
-    <hyperlink ref="G56" r:id="rId40" display="Adactrain@1"/>
-    <hyperlink ref="G57" r:id="rId41" display="Adactrain@1"/>
-    <hyperlink ref="G58" r:id="rId42" display="Adactrain@1"/>
+    <hyperlink ref="G16" r:id="rId1" display="Adactrain@1"/>
+    <hyperlink ref="G17" r:id="rId2" display="Adactrain@1"/>
+    <hyperlink ref="G18" r:id="rId3" display="Adactrain@1"/>
+    <hyperlink ref="G19" r:id="rId4" display="Adactrain@1"/>
+    <hyperlink ref="G20" r:id="rId5" display="Adactrain@1"/>
+    <hyperlink ref="G21" r:id="rId6" display="Adactrain@1"/>
+    <hyperlink ref="G22" r:id="rId7" display="Adactrain@1"/>
+    <hyperlink ref="G23" r:id="rId8" display="Adactrain@1"/>
+    <hyperlink ref="G24" r:id="rId9" display="Adactrain@1"/>
+    <hyperlink ref="G25" r:id="rId10" display="Adactrain@1"/>
+    <hyperlink ref="G26" r:id="rId11" display="Adactrain@1"/>
+    <hyperlink ref="G27" r:id="rId12" display="Adactrain@1"/>
+    <hyperlink ref="G28" r:id="rId13" display="Adactrain@1"/>
+    <hyperlink ref="G29" r:id="rId14" display="Adactrain@1"/>
+    <hyperlink ref="G30" r:id="rId15" display="Adactrain@1"/>
+    <hyperlink ref="G31" r:id="rId16" display="Adactrain@1"/>
+    <hyperlink ref="G32" r:id="rId17" display="Adactrain@1"/>
+    <hyperlink ref="G33" r:id="rId18" display="Adactrain@1"/>
+    <hyperlink ref="G37" r:id="rId19" display="Adactrain@1"/>
+    <hyperlink ref="G38" r:id="rId20" display="Adactrain@1"/>
+    <hyperlink ref="G39" r:id="rId21" display="Adactrain@1"/>
+    <hyperlink ref="G40" r:id="rId22" display="Adactrain@1"/>
+    <hyperlink ref="G41" r:id="rId23" display="Adactrain@1"/>
+    <hyperlink ref="G42" r:id="rId24" display="Adactrain@1"/>
+    <hyperlink ref="G43" r:id="rId25" display="Adactrain@1"/>
+    <hyperlink ref="G44" r:id="rId26" display="Adactrain@1"/>
+    <hyperlink ref="G45" r:id="rId27" display="Adactrain@1"/>
+    <hyperlink ref="G46" r:id="rId28" display="Adactrain@1"/>
+    <hyperlink ref="G47" r:id="rId29" display="Adactrain@1"/>
+    <hyperlink ref="G48" r:id="rId30" display="Adactrain@1"/>
+    <hyperlink ref="G49" r:id="rId31" display="Adactrain@1"/>
+    <hyperlink ref="G50" r:id="rId32" display="Adactrain@1"/>
+    <hyperlink ref="G51" r:id="rId33" display="Adactrain@1"/>
+    <hyperlink ref="G52" r:id="rId34" display="Adactrain@1"/>
+    <hyperlink ref="G53" r:id="rId35" display="Adactrain@1"/>
+    <hyperlink ref="G54" r:id="rId36" display="Adactrain@1"/>
+    <hyperlink ref="G55" r:id="rId37" display="Adactrain@1"/>
+    <hyperlink ref="G56" r:id="rId38" display="Adactrain@1"/>
+    <hyperlink ref="G57" r:id="rId39" display="Adactrain@1"/>
+    <hyperlink ref="G58" r:id="rId40" display="Adactrain@1"/>
+    <hyperlink ref="G59" r:id="rId41" display="Adactrain@1"/>
+    <hyperlink ref="G60" r:id="rId42" display="Adactrain@1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Committing latest modifications - negative scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="147">
   <si>
     <t xml:space="preserve">Test_Case_Name</t>
   </si>
@@ -43,6 +43,12 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
+    <t xml:space="preserve">Email Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Verification Text</t>
+  </si>
+  <si>
     <t xml:space="preserve">Location</t>
   </si>
   <si>
@@ -112,6 +118,12 @@
     <t xml:space="preserve">Error message for blank username</t>
   </si>
   <si>
+    <t xml:space="preserve">Alert message for invalid search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message for invalid search</t>
+  </si>
+  <si>
     <t xml:space="preserve">Error message for blank password</t>
   </si>
   <si>
@@ -139,6 +151,12 @@
     <t xml:space="preserve">User_is_able_to_send_email</t>
   </si>
   <si>
+    <t xml:space="preserve">shweta.hannab@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An email has been sent to your email address containing Username and Password. Please check your email.</t>
+  </si>
+  <si>
     <t xml:space="preserve">User_is_shown_an_error_message_when_he_enters_incorrect_username_or_password</t>
   </si>
   <si>
@@ -161,6 +179,18 @@
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_cancel_a_hotel_booking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_view_error_Search_No_Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shwetabinu1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please provide data for following fields - Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select a valid location</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_Search_Hotel_with_Location</t>
@@ -250,6 +280,9 @@
   </si>
   <si>
     <t xml:space="preserve">Please Enter 16 Digits of Credit Card Number !!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User_is_able_to_view_error_Book_No_Input</t>
   </si>
   <si>
     <t xml:space="preserve">User_is_able_to_view_itinerary</t>
@@ -811,7 +844,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -848,6 +881,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -858,6 +895,10 @@
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -957,13 +998,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG61"/>
+  <dimension ref="A1:AK63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AF4" activeCellId="0" sqref="AF4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="87.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.63"/>
@@ -972,28 +1013,29 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="17.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="17.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="24.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="13.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="27.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="19.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="22.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="29.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="17.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="17.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="24.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="0" width="27.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="33" style="0" width="19.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="22.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="19.08"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="35.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1078,10 +1120,10 @@
       <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
       <c r="AE1" s="2" t="s">
@@ -1093,1837 +1135,2040 @@
       <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E2" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="57.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E3" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="8"/>
+      <c r="H3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E4" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="8"/>
-      <c r="AC4" s="9" t="s">
-        <v>42</v>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="8"/>
+      <c r="AE4" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E5" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="8"/>
-      <c r="AD5" s="0" t="s">
-        <v>44</v>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="8"/>
+      <c r="AF5" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E6" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="8"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="8"/>
-      <c r="X7" s="0" t="n">
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="8"/>
+      <c r="Z7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="47.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E8" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="AC8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="8"/>
+      <c r="AG8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="47.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E9" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>53</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="AE9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M10" s="11" t="n">
-        <v>44026</v>
-      </c>
-      <c r="N10" s="11" t="n">
-        <v>44027</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E11" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>53</v>
+        <v>41</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="M11" s="11" t="n">
-        <v>43919</v>
+        <v>65</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="N11" s="11" t="n">
-        <v>43920</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>59</v>
+        <v>1</v>
+      </c>
+      <c r="O11" s="12" t="n">
+        <v>44026</v>
+      </c>
+      <c r="P11" s="12" t="n">
+        <v>44027</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E12" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="O12" s="12" t="n">
+        <v>43919</v>
+      </c>
+      <c r="P12" s="12" t="n">
+        <v>43920</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E13" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="M13" s="11" t="n">
-        <v>44032</v>
-      </c>
-      <c r="N13" s="11" t="n">
-        <v>44033</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q13" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="R13" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="S13" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="T13" s="12" t="n">
-        <v>1234567891234570</v>
-      </c>
-      <c r="U13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="W13" s="0" t="n">
-        <v>123</v>
-      </c>
-      <c r="X13" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="9" t="s">
+      <c r="M13" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="AG13" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N13" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E14" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L14" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M14" s="11" t="n">
-        <v>44007</v>
-      </c>
-      <c r="N14" s="11" t="n">
-        <v>44008</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q14" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="R14" s="0" t="s">
+      <c r="F14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="Y14" s="0" t="s">
+      <c r="M14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="N14" s="0" t="s">
         <v>69</v>
       </c>
+      <c r="O14" s="12" t="n">
+        <v>44032</v>
+      </c>
+      <c r="P14" s="12" t="n">
+        <v>44033</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="T14" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="U14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="V14" s="14" t="n">
+        <v>1234567891234570</v>
+      </c>
+      <c r="W14" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y14" s="0" t="n">
+        <v>123</v>
+      </c>
       <c r="Z14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB14" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK14" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E15" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L15" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" s="11" t="n">
-        <v>44007</v>
-      </c>
-      <c r="N15" s="11" t="n">
-        <v>44008</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q15" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="R15" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="X15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y15" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB15" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
-        <v>73</v>
+      <c r="F15" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="15"/>
+      <c r="AJ15" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5" t="n">
         <v>10</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>56</v>
+        <v>41</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M16" s="11" t="n">
-        <v>43919</v>
+        <v>63</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="N16" s="11" t="n">
-        <v>43920</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q16" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="R16" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" s="12" t="n">
+        <v>44007</v>
+      </c>
+      <c r="P16" s="12" t="n">
+        <v>44008</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="T16" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA16" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC16" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD16" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="S16" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="T16" s="12" t="n">
-        <v>1234567891234570</v>
-      </c>
-      <c r="U16" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="W16" s="0" t="n">
-        <v>1223</v>
-      </c>
-      <c r="X16" s="4" t="n">
+      <c r="M17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="11" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L17" s="10" t="n">
+      <c r="O17" s="12" t="n">
+        <v>44007</v>
+      </c>
+      <c r="P17" s="12" t="n">
+        <v>44008</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="S17" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="T17" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="M17" s="11" t="n">
-        <v>43975</v>
-      </c>
-      <c r="N17" s="11" t="n">
-        <v>43977</v>
-      </c>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="5" t="n">
-        <v>22</v>
-      </c>
-      <c r="R17" s="5" t="n">
-        <v>33</v>
-      </c>
-      <c r="S17" s="9"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="13"/>
-      <c r="X17" s="10" t="n">
+      <c r="AA17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="Y17" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z17" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA17" s="5" t="s">
+      <c r="AC17" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="AB17" s="5" t="s">
+      <c r="AD17" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="AD17" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="16" t="s">
         <v>84</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>78</v>
+        <v>10</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>86</v>
+      <c r="J18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O18" s="12" t="n">
+        <v>43919</v>
+      </c>
+      <c r="P18" s="12" t="n">
+        <v>43920</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="T18" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="V18" s="14" t="n">
+        <v>1234567891234570</v>
+      </c>
+      <c r="W18" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y18" s="0" t="n">
+        <v>1223</v>
+      </c>
+      <c r="Z18" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="16" t="s">
+        <v>85</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E19" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>78</v>
+      <c r="F19" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>87</v>
+      <c r="J19" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O19" s="12" t="n">
+        <v>43975</v>
+      </c>
+      <c r="P19" s="12" t="n">
+        <v>43977</v>
+      </c>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="T19" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="U19" s="10"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="15"/>
+      <c r="Z19" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB19" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD19" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF19" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="E20" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F20" s="15" t="s">
-        <v>78</v>
+      <c r="F20" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I20" s="14"/>
-    </row>
-    <row r="21" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="E21" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F21" s="15" t="s">
-        <v>78</v>
+      <c r="F21" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="s">
-        <v>91</v>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="87.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="E22" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F22" s="15" t="s">
-        <v>78</v>
+      <c r="F22" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
-        <v>93</v>
+        <v>90</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="K22" s="16"/>
+    </row>
+    <row r="23" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="E23" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>78</v>
+      <c r="F23" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="E24" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F24" s="15" t="s">
-        <v>78</v>
+      <c r="F24" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="M24" s="11" t="n">
+        <v>90</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="M24" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="N25" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="O26" s="12" t="n">
         <v>43919</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="9" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="M25" s="11" t="n">
+      <c r="E27" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="O27" s="12" t="n">
         <v>43919</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="M26" s="11" t="n">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="O28" s="12" t="n">
         <v>43919</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="N27" s="11" t="n">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="P29" s="12" t="n">
         <v>43920</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="N28" s="11" t="n">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="P30" s="12" t="n">
         <v>43920</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E29" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="N29" s="11" t="n">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="P31" s="12" t="n">
         <v>43920</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O30" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E31" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="P31" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9" t="s">
-        <v>105</v>
+    <row r="32" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10" t="s">
+        <v>112</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E32" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F32" s="15" t="s">
-        <v>78</v>
+      <c r="F32" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
-        <v>106</v>
+        <v>90</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="Q32" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E33" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F33" s="15" t="s">
-        <v>78</v>
+      <c r="F33" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>79</v>
+        <v>90</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="R33" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
-        <v>107</v>
+      <c r="A34" s="10" t="s">
+        <v>116</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E34" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F34" s="15" t="s">
-        <v>78</v>
+      <c r="F34" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9" t="s">
-        <v>108</v>
+      <c r="A35" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E35" s="5" t="n">
         <v>13.3</v>
       </c>
+      <c r="F35" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
-        <v>109</v>
+      <c r="A36" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E36" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F36" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="G36" s="0" t="n">
+      <c r="F36" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="5" t="n">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="G38" s="0" t="n">
         <v>123344</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="5" t="n">
-        <v>13.3</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M38" s="11" t="n">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E40" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="O40" s="12" t="n">
         <v>43919</v>
       </c>
-      <c r="N38" s="11" t="n">
+      <c r="P40" s="12" t="n">
         <v>43920</v>
       </c>
-      <c r="O38" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="P38" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E39" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" s="5" t="n">
-        <v>13.3</v>
-      </c>
-      <c r="F40" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>79</v>
+      <c r="Q40" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="R40" s="4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9" t="s">
-        <v>115</v>
+      <c r="A41" s="10" t="s">
+        <v>124</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E41" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F41" s="15" t="s">
-        <v>78</v>
+      <c r="F41" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9" t="s">
-        <v>116</v>
+      <c r="A42" s="10" t="s">
+        <v>125</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E42" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F42" s="15" t="s">
-        <v>78</v>
+      <c r="F42" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9" t="s">
-        <v>117</v>
+      <c r="A43" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E43" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F43" s="15" t="s">
-        <v>78</v>
+      <c r="F43" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
-        <v>118</v>
+      <c r="A44" s="10" t="s">
+        <v>127</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E44" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F44" s="15" t="s">
-        <v>78</v>
+      <c r="F44" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="9" t="s">
-        <v>119</v>
+        <v>90</v>
+      </c>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E45" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F45" s="15" t="s">
-        <v>78</v>
+      <c r="F45" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="9" t="s">
-        <v>120</v>
+      <c r="A46" s="10" t="s">
+        <v>129</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E46" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F46" s="15" t="s">
-        <v>78</v>
+      <c r="F46" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="9" t="s">
-        <v>121</v>
+        <v>90</v>
+      </c>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="10" t="s">
+        <v>130</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E47" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F47" s="15" t="s">
-        <v>78</v>
+      <c r="F47" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
-        <v>122</v>
+      <c r="A48" s="10" t="s">
+        <v>131</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E48" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F48" s="15" t="s">
-        <v>78</v>
+      <c r="F48" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="s">
-        <v>123</v>
+      <c r="A49" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E49" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F49" s="15" t="s">
-        <v>78</v>
+      <c r="F49" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="9" t="s">
-        <v>124</v>
+      <c r="A50" s="10" t="s">
+        <v>133</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E50" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F50" s="15" t="s">
-        <v>78</v>
+      <c r="F50" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9" t="s">
-        <v>125</v>
+      <c r="A51" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E51" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F51" s="15" t="s">
-        <v>78</v>
+      <c r="F51" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I51" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="s">
-        <v>126</v>
+      <c r="A52" s="10" t="s">
+        <v>135</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E52" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F52" s="15" t="s">
-        <v>78</v>
+      <c r="F52" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="I52" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9" t="s">
-        <v>128</v>
+      <c r="A53" s="10" t="s">
+        <v>136</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E53" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F53" s="15" t="s">
-        <v>78</v>
+      <c r="F53" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H53" s="0" t="s">
-        <v>129</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9" t="s">
-        <v>130</v>
+      <c r="A54" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E54" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F54" s="15" t="s">
-        <v>78</v>
+      <c r="F54" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="K54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
-        <v>131</v>
+      <c r="A55" s="10" t="s">
+        <v>139</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E55" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F55" s="15" t="s">
-        <v>78</v>
+      <c r="F55" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="I55" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="0" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9" t="s">
-        <v>133</v>
+      <c r="A56" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E56" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F56" s="15" t="s">
-        <v>78</v>
+      <c r="F56" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="s">
-        <v>124</v>
+      <c r="A57" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E57" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F57" s="15" t="s">
-        <v>78</v>
+      <c r="F57" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K57" s="4"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9" t="s">
-        <v>134</v>
+      <c r="A58" s="10" t="s">
+        <v>144</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E58" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F58" s="15" t="s">
-        <v>78</v>
+      <c r="F58" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="10" t="s">
         <v>135</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E59" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F59" s="15" t="s">
-        <v>78</v>
+      <c r="F59" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="10" t="s">
+        <v>145</v>
+      </c>
       <c r="B60" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E60" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F60" s="15" t="s">
-        <v>78</v>
+      <c r="F60" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="10" t="s">
+        <v>146</v>
+      </c>
       <c r="B61" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E61" s="5" t="n">
         <v>13.3</v>
       </c>
-      <c r="F61" s="15" t="s">
-        <v>78</v>
+      <c r="F61" s="17" t="s">
+        <v>89</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>79</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E62" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E63" s="5" t="n">
+        <v>13.3</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G17" r:id="rId1" display="Adactrain@1"/>
-    <hyperlink ref="G18" r:id="rId2" display="Adactrain@1"/>
-    <hyperlink ref="G19" r:id="rId3" display="Adactrain@1"/>
-    <hyperlink ref="G20" r:id="rId4" display="Adactrain@1"/>
-    <hyperlink ref="G21" r:id="rId5" display="Adactrain@1"/>
-    <hyperlink ref="G22" r:id="rId6" display="Adactrain@1"/>
-    <hyperlink ref="G23" r:id="rId7" display="Adactrain@1"/>
-    <hyperlink ref="G24" r:id="rId8" display="Adactrain@1"/>
-    <hyperlink ref="G25" r:id="rId9" display="Adactrain@1"/>
-    <hyperlink ref="G26" r:id="rId10" display="Adactrain@1"/>
-    <hyperlink ref="G27" r:id="rId11" display="Adactrain@1"/>
-    <hyperlink ref="G28" r:id="rId12" display="Adactrain@1"/>
-    <hyperlink ref="G29" r:id="rId13" display="Adactrain@1"/>
-    <hyperlink ref="G30" r:id="rId14" display="Adactrain@1"/>
-    <hyperlink ref="G31" r:id="rId15" display="Adactrain@1"/>
-    <hyperlink ref="G32" r:id="rId16" display="Adactrain@1"/>
-    <hyperlink ref="G33" r:id="rId17" display="Adactrain@1"/>
-    <hyperlink ref="G34" r:id="rId18" display="Adactrain@1"/>
-    <hyperlink ref="G38" r:id="rId19" display="Adactrain@1"/>
-    <hyperlink ref="G39" r:id="rId20" display="Adactrain@1"/>
-    <hyperlink ref="G40" r:id="rId21" display="Adactrain@1"/>
-    <hyperlink ref="G41" r:id="rId22" display="Adactrain@1"/>
-    <hyperlink ref="G42" r:id="rId23" display="Adactrain@1"/>
-    <hyperlink ref="G43" r:id="rId24" display="Adactrain@1"/>
-    <hyperlink ref="G44" r:id="rId25" display="Adactrain@1"/>
-    <hyperlink ref="G45" r:id="rId26" display="Adactrain@1"/>
-    <hyperlink ref="G46" r:id="rId27" display="Adactrain@1"/>
-    <hyperlink ref="G47" r:id="rId28" display="Adactrain@1"/>
-    <hyperlink ref="G48" r:id="rId29" display="Adactrain@1"/>
-    <hyperlink ref="G49" r:id="rId30" display="Adactrain@1"/>
-    <hyperlink ref="G50" r:id="rId31" display="Adactrain@1"/>
-    <hyperlink ref="G51" r:id="rId32" display="Adactrain@1"/>
-    <hyperlink ref="G52" r:id="rId33" display="Adactrain@1"/>
-    <hyperlink ref="G53" r:id="rId34" display="Adactrain@1"/>
-    <hyperlink ref="G54" r:id="rId35" display="Adactrain@1"/>
-    <hyperlink ref="G55" r:id="rId36" display="Adactrain@1"/>
-    <hyperlink ref="G56" r:id="rId37" display="Adactrain@1"/>
-    <hyperlink ref="G57" r:id="rId38" display="Adactrain@1"/>
-    <hyperlink ref="G58" r:id="rId39" display="Adactrain@1"/>
-    <hyperlink ref="G59" r:id="rId40" display="Adactrain@1"/>
-    <hyperlink ref="G60" r:id="rId41" display="Adactrain@1"/>
-    <hyperlink ref="G61" r:id="rId42" display="Adactrain@1"/>
+    <hyperlink ref="G19" r:id="rId1" display="Adactrain@1"/>
+    <hyperlink ref="G20" r:id="rId2" display="Adactrain@1"/>
+    <hyperlink ref="G21" r:id="rId3" display="Adactrain@1"/>
+    <hyperlink ref="G22" r:id="rId4" display="Adactrain@1"/>
+    <hyperlink ref="G23" r:id="rId5" display="Adactrain@1"/>
+    <hyperlink ref="G24" r:id="rId6" display="Adactrain@1"/>
+    <hyperlink ref="G25" r:id="rId7" display="Adactrain@1"/>
+    <hyperlink ref="G26" r:id="rId8" display="Adactrain@1"/>
+    <hyperlink ref="G27" r:id="rId9" display="Adactrain@1"/>
+    <hyperlink ref="G28" r:id="rId10" display="Adactrain@1"/>
+    <hyperlink ref="G29" r:id="rId11" display="Adactrain@1"/>
+    <hyperlink ref="G30" r:id="rId12" display="Adactrain@1"/>
+    <hyperlink ref="G31" r:id="rId13" display="Adactrain@1"/>
+    <hyperlink ref="G32" r:id="rId14" display="Adactrain@1"/>
+    <hyperlink ref="G33" r:id="rId15" display="Adactrain@1"/>
+    <hyperlink ref="G34" r:id="rId16" display="Adactrain@1"/>
+    <hyperlink ref="G35" r:id="rId17" display="Adactrain@1"/>
+    <hyperlink ref="G36" r:id="rId18" display="Adactrain@1"/>
+    <hyperlink ref="G40" r:id="rId19" display="Adactrain@1"/>
+    <hyperlink ref="G41" r:id="rId20" display="Adactrain@1"/>
+    <hyperlink ref="G42" r:id="rId21" display="Adactrain@1"/>
+    <hyperlink ref="G43" r:id="rId22" display="Adactrain@1"/>
+    <hyperlink ref="G44" r:id="rId23" display="Adactrain@1"/>
+    <hyperlink ref="G45" r:id="rId24" display="Adactrain@1"/>
+    <hyperlink ref="G46" r:id="rId25" display="Adactrain@1"/>
+    <hyperlink ref="G47" r:id="rId26" display="Adactrain@1"/>
+    <hyperlink ref="G48" r:id="rId27" display="Adactrain@1"/>
+    <hyperlink ref="G49" r:id="rId28" display="Adactrain@1"/>
+    <hyperlink ref="G50" r:id="rId29" display="Adactrain@1"/>
+    <hyperlink ref="G51" r:id="rId30" display="Adactrain@1"/>
+    <hyperlink ref="G52" r:id="rId31" display="Adactrain@1"/>
+    <hyperlink ref="G53" r:id="rId32" display="Adactrain@1"/>
+    <hyperlink ref="G54" r:id="rId33" display="Adactrain@1"/>
+    <hyperlink ref="G55" r:id="rId34" display="Adactrain@1"/>
+    <hyperlink ref="G56" r:id="rId35" display="Adactrain@1"/>
+    <hyperlink ref="G57" r:id="rId36" display="Adactrain@1"/>
+    <hyperlink ref="G58" r:id="rId37" display="Adactrain@1"/>
+    <hyperlink ref="G59" r:id="rId38" display="Adactrain@1"/>
+    <hyperlink ref="G60" r:id="rId39" display="Adactrain@1"/>
+    <hyperlink ref="G61" r:id="rId40" display="Adactrain@1"/>
+    <hyperlink ref="G62" r:id="rId41" display="Adactrain@1"/>
+    <hyperlink ref="G63" r:id="rId42" display="Adactrain@1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>